<commit_message>
feat: add general admissions table
</commit_message>
<xml_diff>
--- a/tables/Pneumonia_data_by_age_group_08.11.xlsx
+++ b/tables/Pneumonia_data_by_age_group_08.11.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Age_groups" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,6 +14,7 @@
     <sheet name="Los_ICU Age_group" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Cids ranking" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="CIDS_description" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Age_groups_ICU_General" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="229">
   <si>
     <t xml:space="preserve">Data Information</t>
   </si>
@@ -1115,19 +1116,27 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="9" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="9" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1158,10 +1167,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1183,10 +1188,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1316,7 +1317,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4895280" y="424440"/>
+          <a:off x="4896360" y="424440"/>
           <a:ext cx="1242720" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1358,7 +1359,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4895280" y="572040"/>
+          <a:off x="4896360" y="572040"/>
           <a:ext cx="1248120" cy="162360"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1400,7 +1401,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4881240" y="722880"/>
+          <a:off x="4882320" y="722880"/>
           <a:ext cx="1249920" cy="330840"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1442,7 +1443,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="4881600" y="897120"/>
+          <a:off x="4882680" y="897120"/>
           <a:ext cx="1261800" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1484,7 +1485,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="4886280" y="565920"/>
+          <a:off x="4887360" y="565920"/>
           <a:ext cx="1257120" cy="493560"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1526,7 +1527,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4892400" y="1710720"/>
+          <a:off x="4893480" y="1710720"/>
           <a:ext cx="1248120" cy="162360"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1568,7 +1569,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4892040" y="1216080"/>
+          <a:off x="4893120" y="1216080"/>
           <a:ext cx="1242720" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1610,7 +1611,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4892040" y="1378080"/>
+          <a:off x="4893120" y="1378080"/>
           <a:ext cx="1242720" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1652,7 +1653,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4898520" y="1535040"/>
+          <a:off x="4899600" y="1535040"/>
           <a:ext cx="1242720" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1694,7 +1695,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4887360" y="1885680"/>
+          <a:off x="4888440" y="1885680"/>
           <a:ext cx="321480" cy="408240"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1736,7 +1737,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="5719320" y="1710360"/>
+          <a:off x="5720400" y="1710360"/>
           <a:ext cx="423720" cy="595440"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1767,9 +1768,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>922680</xdr:colOff>
+      <xdr:colOff>922320</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>124560</xdr:rowOff>
+      <xdr:rowOff>124200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1778,8 +1779,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5544360" y="2311560"/>
-          <a:ext cx="259560" cy="263880"/>
+          <a:off x="5545440" y="2311560"/>
+          <a:ext cx="259200" cy="263520"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1843,8 +1844,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10809720" y="390960"/>
-          <a:ext cx="1247760" cy="0"/>
+          <a:off x="10810800" y="390960"/>
+          <a:ext cx="1249200" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1885,8 +1886,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10809720" y="897480"/>
-          <a:ext cx="1247760" cy="0"/>
+          <a:off x="10810800" y="897480"/>
+          <a:ext cx="1249200" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1927,8 +1928,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10809720" y="565920"/>
-          <a:ext cx="1247760" cy="0"/>
+          <a:off x="10810800" y="565920"/>
+          <a:ext cx="1249200" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1969,8 +1970,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10821960" y="722160"/>
-          <a:ext cx="1247760" cy="0"/>
+          <a:off x="10823040" y="722160"/>
+          <a:ext cx="1249200" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2011,8 +2012,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10821960" y="1535040"/>
-          <a:ext cx="1247760" cy="0"/>
+          <a:off x="10823040" y="1535040"/>
+          <a:ext cx="1249200" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2053,8 +2054,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="10821960" y="1053720"/>
-          <a:ext cx="1240920" cy="662400"/>
+          <a:off x="10823040" y="1053720"/>
+          <a:ext cx="1242360" cy="662400"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2095,8 +2096,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10821960" y="1047240"/>
-          <a:ext cx="1240920" cy="174960"/>
+          <a:off x="10823040" y="1047240"/>
+          <a:ext cx="1242360" cy="174960"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2137,8 +2138,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10821960" y="1209960"/>
-          <a:ext cx="1253880" cy="162720"/>
+          <a:off x="10823040" y="1209960"/>
+          <a:ext cx="1255320" cy="162720"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2179,8 +2180,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10822320" y="1860120"/>
-          <a:ext cx="384120" cy="390960"/>
+          <a:off x="10823400" y="1860120"/>
+          <a:ext cx="385560" cy="390960"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2221,8 +2222,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10822320" y="1372320"/>
-          <a:ext cx="1220400" cy="318240"/>
+          <a:off x="10823400" y="1372320"/>
+          <a:ext cx="1221840" cy="318240"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2263,7 +2264,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="11682000" y="1847880"/>
+          <a:off x="11684520" y="1847880"/>
           <a:ext cx="386280" cy="411480"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2294,9 +2295,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>481320</xdr:colOff>
+      <xdr:colOff>480960</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>107280</xdr:rowOff>
+      <xdr:rowOff>106920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2305,8 +2306,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5103000" y="2294280"/>
-          <a:ext cx="259560" cy="263880"/>
+          <a:off x="5104080" y="2294280"/>
+          <a:ext cx="259200" cy="263520"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -2359,9 +2360,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>535320</xdr:colOff>
+      <xdr:colOff>534960</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>62640</xdr:rowOff>
+      <xdr:rowOff>62280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2370,8 +2371,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11108160" y="2249640"/>
-          <a:ext cx="259560" cy="263880"/>
+          <a:off x="11110680" y="2249640"/>
+          <a:ext cx="259200" cy="263520"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -2424,9 +2425,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>994320</xdr:colOff>
+      <xdr:colOff>993960</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>75240</xdr:rowOff>
+      <xdr:rowOff>74880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2435,8 +2436,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11567160" y="2262240"/>
-          <a:ext cx="259560" cy="263880"/>
+          <a:off x="11569680" y="2262240"/>
+          <a:ext cx="259200" cy="263520"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -2494,7 +2495,7 @@
       <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="2" style="0" width="10.84"/>
@@ -4516,7 +4517,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="0" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
@@ -4535,9 +4536,9 @@
       <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="2" style="0" width="10.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.8"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="15" min="13" style="0" width="10.84"/>
@@ -5663,7 +5664,7 @@
         <v>-25.487374034126</v>
       </c>
     </row>
-    <row r="17" s="41" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" s="41" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="19" t="s">
         <v>11</v>
       </c>
@@ -6015,7 +6016,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="46" t="s">
         <v>16</v>
       </c>
       <c r="B22" s="11" t="n">
@@ -6225,7 +6226,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="44" t="s">
+      <c r="A25" s="46" t="s">
         <v>16</v>
       </c>
       <c r="B25" s="11" t="n">
@@ -6435,7 +6436,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="44" t="s">
+      <c r="A28" s="46" t="s">
         <v>16</v>
       </c>
       <c r="B28" s="11" t="n">
@@ -6575,34 +6576,34 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="46" t="s">
+      <c r="A30" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="47" t="s">
+      <c r="B30" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="47" t="s">
+      <c r="C30" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="D30" s="47" t="s">
+      <c r="D30" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="E30" s="47" t="s">
+      <c r="E30" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="F30" s="47" t="s">
+      <c r="F30" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="G30" s="47" t="s">
+      <c r="G30" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="H30" s="47" t="s">
+      <c r="H30" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="I30" s="47" t="s">
+      <c r="I30" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="J30" s="47" t="s">
+      <c r="J30" s="48" t="s">
         <v>69</v>
       </c>
       <c r="K30" s="28" t="n">
@@ -6621,10 +6622,10 @@
       <c r="O30" s="28" t="n">
         <v>1.49808694638598</v>
       </c>
-      <c r="P30" s="47" t="s">
+      <c r="P30" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="Q30" s="47" t="s">
+      <c r="Q30" s="48" t="s">
         <v>71</v>
       </c>
       <c r="R30" s="28" t="n">
@@ -6645,7 +6646,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="46" t="s">
+      <c r="A31" s="49" t="s">
         <v>16</v>
       </c>
       <c r="B31" s="27" t="n">
@@ -6736,17 +6737,17 @@
       <c r="B34" s="35"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="48"/>
-      <c r="C35" s="48"/>
-      <c r="D35" s="48"/>
-      <c r="E35" s="48"/>
-      <c r="F35" s="48"/>
-      <c r="G35" s="48"/>
-      <c r="H35" s="48"/>
-      <c r="I35" s="48"/>
-      <c r="J35" s="48"/>
-      <c r="P35" s="48"/>
-      <c r="Q35" s="48"/>
+      <c r="B35" s="50"/>
+      <c r="C35" s="50"/>
+      <c r="D35" s="50"/>
+      <c r="E35" s="50"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="50"/>
+      <c r="H35" s="50"/>
+      <c r="I35" s="50"/>
+      <c r="J35" s="50"/>
+      <c r="P35" s="50"/>
+      <c r="Q35" s="50"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="45"/>
@@ -6827,15 +6828,15 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="48"/>
-      <c r="C38" s="48"/>
-      <c r="D38" s="48"/>
-      <c r="E38" s="48"/>
-      <c r="F38" s="48"/>
-      <c r="G38" s="48"/>
-      <c r="H38" s="48"/>
-      <c r="I38" s="48"/>
-      <c r="J38" s="48"/>
+      <c r="B38" s="50"/>
+      <c r="C38" s="50"/>
+      <c r="D38" s="50"/>
+      <c r="E38" s="50"/>
+      <c r="F38" s="50"/>
+      <c r="G38" s="50"/>
+      <c r="H38" s="50"/>
+      <c r="I38" s="50"/>
+      <c r="J38" s="50"/>
       <c r="K38" s="45"/>
       <c r="L38" s="45"/>
       <c r="M38" s="45" t="str">
@@ -6850,8 +6851,8 @@
         <f aca="false">SUBSTITUTE(ROUND(O4,2),",",".")</f>
         <v>-0.38</v>
       </c>
-      <c r="P38" s="48"/>
-      <c r="Q38" s="48"/>
+      <c r="P38" s="50"/>
+      <c r="Q38" s="50"/>
       <c r="T38" s="45" t="str">
         <f aca="false">SUBSTITUTE(ROUND(T4,2),",",".")</f>
         <v>-22.72</v>
@@ -6905,17 +6906,17 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="49"/>
-      <c r="C40" s="49"/>
-      <c r="D40" s="49"/>
-      <c r="E40" s="49"/>
-      <c r="F40" s="49"/>
-      <c r="G40" s="49"/>
-      <c r="H40" s="49"/>
-      <c r="I40" s="49"/>
-      <c r="J40" s="49"/>
-      <c r="K40" s="49"/>
-      <c r="L40" s="49"/>
+      <c r="B40" s="51"/>
+      <c r="C40" s="51"/>
+      <c r="D40" s="51"/>
+      <c r="E40" s="51"/>
+      <c r="F40" s="51"/>
+      <c r="G40" s="51"/>
+      <c r="H40" s="51"/>
+      <c r="I40" s="51"/>
+      <c r="J40" s="51"/>
+      <c r="K40" s="51"/>
+      <c r="L40" s="51"/>
       <c r="M40" s="45" t="str">
         <f aca="false">SUBSTITUTE(ROUND(M6,2),",",".")</f>
         <v>1.49</v>
@@ -6928,8 +6929,8 @@
         <f aca="false">SUBSTITUTE(ROUND(O6,2),",",".")</f>
         <v>1.93</v>
       </c>
-      <c r="P40" s="49"/>
-      <c r="Q40" s="49"/>
+      <c r="P40" s="51"/>
+      <c r="Q40" s="51"/>
       <c r="T40" s="45" t="str">
         <f aca="false">SUBSTITUTE(ROUND(T6,2),",",".")</f>
         <v>3.52</v>
@@ -6944,17 +6945,17 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="48"/>
-      <c r="C41" s="48"/>
-      <c r="D41" s="48"/>
-      <c r="E41" s="48"/>
-      <c r="F41" s="48"/>
-      <c r="G41" s="48"/>
-      <c r="H41" s="48"/>
-      <c r="I41" s="48"/>
-      <c r="J41" s="48"/>
-      <c r="K41" s="49"/>
-      <c r="L41" s="49"/>
+      <c r="B41" s="50"/>
+      <c r="C41" s="50"/>
+      <c r="D41" s="50"/>
+      <c r="E41" s="50"/>
+      <c r="F41" s="50"/>
+      <c r="G41" s="50"/>
+      <c r="H41" s="50"/>
+      <c r="I41" s="50"/>
+      <c r="J41" s="50"/>
+      <c r="K41" s="51"/>
+      <c r="L41" s="51"/>
       <c r="M41" s="45" t="str">
         <f aca="false">SUBSTITUTE(ROUND(M7,2),",",".")</f>
         <v>-6.16</v>
@@ -6967,8 +6968,8 @@
         <f aca="false">SUBSTITUTE(ROUND(O7,2),",",".")</f>
         <v>-6.08</v>
       </c>
-      <c r="P41" s="48"/>
-      <c r="Q41" s="48"/>
+      <c r="P41" s="50"/>
+      <c r="Q41" s="50"/>
       <c r="T41" s="45" t="str">
         <f aca="false">SUBSTITUTE(ROUND(T7,2),",",".")</f>
         <v>-17.36</v>
@@ -6992,8 +6993,8 @@
       <c r="H42" s="45"/>
       <c r="I42" s="45"/>
       <c r="J42" s="45"/>
-      <c r="K42" s="49"/>
-      <c r="L42" s="49"/>
+      <c r="K42" s="51"/>
+      <c r="L42" s="51"/>
       <c r="M42" s="45" t="str">
         <f aca="false">SUBSTITUTE(ROUND(M8,2),",",".")</f>
         <v>-2.06</v>
@@ -7022,17 +7023,17 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="49"/>
-      <c r="C43" s="49"/>
-      <c r="D43" s="49"/>
-      <c r="E43" s="49"/>
-      <c r="F43" s="49"/>
-      <c r="G43" s="49"/>
-      <c r="H43" s="49"/>
-      <c r="I43" s="49"/>
-      <c r="J43" s="49"/>
-      <c r="K43" s="49"/>
-      <c r="L43" s="49"/>
+      <c r="B43" s="51"/>
+      <c r="C43" s="51"/>
+      <c r="D43" s="51"/>
+      <c r="E43" s="51"/>
+      <c r="F43" s="51"/>
+      <c r="G43" s="51"/>
+      <c r="H43" s="51"/>
+      <c r="I43" s="51"/>
+      <c r="J43" s="51"/>
+      <c r="K43" s="51"/>
+      <c r="L43" s="51"/>
       <c r="M43" s="45" t="str">
         <f aca="false">SUBSTITUTE(ROUND(M9,2),",",".")</f>
         <v>3.34</v>
@@ -7045,8 +7046,8 @@
         <f aca="false">SUBSTITUTE(ROUND(O9,2),",",".")</f>
         <v>3.86</v>
       </c>
-      <c r="P43" s="49"/>
-      <c r="Q43" s="49"/>
+      <c r="P43" s="51"/>
+      <c r="Q43" s="51"/>
       <c r="T43" s="45" t="str">
         <f aca="false">SUBSTITUTE(ROUND(T9,2),",",".")</f>
         <v>5.61</v>
@@ -7061,17 +7062,17 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="48"/>
-      <c r="C44" s="48"/>
-      <c r="D44" s="48"/>
-      <c r="E44" s="48"/>
-      <c r="F44" s="48"/>
-      <c r="G44" s="48"/>
-      <c r="H44" s="48"/>
-      <c r="I44" s="48"/>
-      <c r="J44" s="48"/>
-      <c r="K44" s="49"/>
-      <c r="L44" s="49"/>
+      <c r="B44" s="50"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="50"/>
+      <c r="E44" s="50"/>
+      <c r="F44" s="50"/>
+      <c r="G44" s="50"/>
+      <c r="H44" s="50"/>
+      <c r="I44" s="50"/>
+      <c r="J44" s="50"/>
+      <c r="K44" s="51"/>
+      <c r="L44" s="51"/>
       <c r="M44" s="45" t="str">
         <f aca="false">SUBSTITUTE(ROUND(M10,2),",",".")</f>
         <v>-2.39</v>
@@ -7084,8 +7085,8 @@
         <f aca="false">SUBSTITUTE(ROUND(O10,2),",",".")</f>
         <v>-2.27</v>
       </c>
-      <c r="P44" s="48"/>
-      <c r="Q44" s="48"/>
+      <c r="P44" s="50"/>
+      <c r="Q44" s="50"/>
       <c r="T44" s="45" t="str">
         <f aca="false">SUBSTITUTE(ROUND(T10,2),",",".")</f>
         <v>-18.91</v>
@@ -7109,8 +7110,8 @@
       <c r="H45" s="45"/>
       <c r="I45" s="45"/>
       <c r="J45" s="45"/>
-      <c r="K45" s="49"/>
-      <c r="L45" s="49"/>
+      <c r="K45" s="51"/>
+      <c r="L45" s="51"/>
       <c r="M45" s="45" t="str">
         <f aca="false">SUBSTITUTE(ROUND(M11,2),",",".")</f>
         <v>0.95</v>
@@ -7139,17 +7140,17 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="49"/>
-      <c r="C46" s="49"/>
-      <c r="D46" s="49"/>
-      <c r="E46" s="49"/>
-      <c r="F46" s="49"/>
-      <c r="G46" s="49"/>
-      <c r="H46" s="49"/>
-      <c r="I46" s="49"/>
-      <c r="J46" s="49"/>
-      <c r="K46" s="49"/>
-      <c r="L46" s="49"/>
+      <c r="B46" s="51"/>
+      <c r="C46" s="51"/>
+      <c r="D46" s="51"/>
+      <c r="E46" s="51"/>
+      <c r="F46" s="51"/>
+      <c r="G46" s="51"/>
+      <c r="H46" s="51"/>
+      <c r="I46" s="51"/>
+      <c r="J46" s="51"/>
+      <c r="K46" s="51"/>
+      <c r="L46" s="51"/>
       <c r="M46" s="45" t="str">
         <f aca="false">SUBSTITUTE(ROUND(M12,2),",",".")</f>
         <v>5.67</v>
@@ -7162,8 +7163,8 @@
         <f aca="false">SUBSTITUTE(ROUND(O12,2),",",".")</f>
         <v>6.12</v>
       </c>
-      <c r="P46" s="49"/>
-      <c r="Q46" s="49"/>
+      <c r="P46" s="51"/>
+      <c r="Q46" s="51"/>
       <c r="T46" s="45" t="str">
         <f aca="false">SUBSTITUTE(ROUND(T12,2),",",".")</f>
         <v>-0.79</v>
@@ -7178,17 +7179,17 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="48"/>
-      <c r="C47" s="48"/>
-      <c r="D47" s="48"/>
-      <c r="E47" s="48"/>
-      <c r="F47" s="48"/>
-      <c r="G47" s="48"/>
-      <c r="H47" s="48"/>
-      <c r="I47" s="48"/>
-      <c r="J47" s="48"/>
-      <c r="K47" s="49"/>
-      <c r="L47" s="49"/>
+      <c r="B47" s="50"/>
+      <c r="C47" s="50"/>
+      <c r="D47" s="50"/>
+      <c r="E47" s="50"/>
+      <c r="F47" s="50"/>
+      <c r="G47" s="50"/>
+      <c r="H47" s="50"/>
+      <c r="I47" s="50"/>
+      <c r="J47" s="50"/>
+      <c r="K47" s="51"/>
+      <c r="L47" s="51"/>
       <c r="M47" s="45" t="str">
         <f aca="false">SUBSTITUTE(ROUND(M13,2),",",".")</f>
         <v>0.64</v>
@@ -7201,8 +7202,8 @@
         <f aca="false">SUBSTITUTE(ROUND(O13,2),",",".")</f>
         <v>0.75</v>
       </c>
-      <c r="P47" s="48"/>
-      <c r="Q47" s="48"/>
+      <c r="P47" s="50"/>
+      <c r="Q47" s="50"/>
       <c r="T47" s="45" t="str">
         <f aca="false">SUBSTITUTE(ROUND(T13,2),",",".")</f>
         <v>-22.45</v>
@@ -7226,8 +7227,8 @@
       <c r="H48" s="45"/>
       <c r="I48" s="45"/>
       <c r="J48" s="45"/>
-      <c r="K48" s="49"/>
-      <c r="L48" s="49"/>
+      <c r="K48" s="51"/>
+      <c r="L48" s="51"/>
       <c r="M48" s="45" t="str">
         <f aca="false">SUBSTITUTE(ROUND(M14,2),",",".")</f>
         <v>2.73</v>
@@ -7256,17 +7257,17 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="49"/>
-      <c r="C49" s="49"/>
-      <c r="D49" s="49"/>
-      <c r="E49" s="49"/>
-      <c r="F49" s="49"/>
-      <c r="G49" s="49"/>
-      <c r="H49" s="49"/>
-      <c r="I49" s="49"/>
-      <c r="J49" s="49"/>
-      <c r="K49" s="49"/>
-      <c r="L49" s="49"/>
+      <c r="B49" s="51"/>
+      <c r="C49" s="51"/>
+      <c r="D49" s="51"/>
+      <c r="E49" s="51"/>
+      <c r="F49" s="51"/>
+      <c r="G49" s="51"/>
+      <c r="H49" s="51"/>
+      <c r="I49" s="51"/>
+      <c r="J49" s="51"/>
+      <c r="K49" s="51"/>
+      <c r="L49" s="51"/>
       <c r="M49" s="45" t="str">
         <f aca="false">SUBSTITUTE(ROUND(M15,2),",",".")</f>
         <v>4.18</v>
@@ -7295,17 +7296,17 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="49"/>
-      <c r="C50" s="49"/>
-      <c r="D50" s="49"/>
-      <c r="E50" s="49"/>
-      <c r="F50" s="49"/>
-      <c r="G50" s="49"/>
-      <c r="H50" s="49"/>
-      <c r="I50" s="49"/>
-      <c r="J50" s="49"/>
-      <c r="K50" s="49"/>
-      <c r="L50" s="49"/>
+      <c r="B50" s="51"/>
+      <c r="C50" s="51"/>
+      <c r="D50" s="51"/>
+      <c r="E50" s="51"/>
+      <c r="F50" s="51"/>
+      <c r="G50" s="51"/>
+      <c r="H50" s="51"/>
+      <c r="I50" s="51"/>
+      <c r="J50" s="51"/>
+      <c r="K50" s="51"/>
+      <c r="L50" s="51"/>
       <c r="M50" s="45" t="str">
         <f aca="false">SUBSTITUTE(ROUND(M16,2),",",".")</f>
         <v>2.64</v>
@@ -7334,17 +7335,17 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="49"/>
-      <c r="C51" s="49"/>
-      <c r="D51" s="49"/>
-      <c r="E51" s="49"/>
-      <c r="F51" s="49"/>
-      <c r="G51" s="49"/>
-      <c r="H51" s="49"/>
-      <c r="I51" s="49"/>
-      <c r="J51" s="49"/>
-      <c r="K51" s="49"/>
-      <c r="L51" s="49"/>
+      <c r="B51" s="51"/>
+      <c r="C51" s="51"/>
+      <c r="D51" s="51"/>
+      <c r="E51" s="51"/>
+      <c r="F51" s="51"/>
+      <c r="G51" s="51"/>
+      <c r="H51" s="51"/>
+      <c r="I51" s="51"/>
+      <c r="J51" s="51"/>
+      <c r="K51" s="51"/>
+      <c r="L51" s="51"/>
       <c r="M51" s="45" t="str">
         <f aca="false">SUBSTITUTE(ROUND(M17,2),",",".")</f>
         <v>-3.26</v>
@@ -7373,17 +7374,17 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="49"/>
-      <c r="C52" s="49"/>
-      <c r="D52" s="49"/>
-      <c r="E52" s="49"/>
-      <c r="F52" s="49"/>
-      <c r="G52" s="49"/>
-      <c r="H52" s="49"/>
-      <c r="I52" s="49"/>
-      <c r="J52" s="49"/>
-      <c r="K52" s="49"/>
-      <c r="L52" s="49"/>
+      <c r="B52" s="51"/>
+      <c r="C52" s="51"/>
+      <c r="D52" s="51"/>
+      <c r="E52" s="51"/>
+      <c r="F52" s="51"/>
+      <c r="G52" s="51"/>
+      <c r="H52" s="51"/>
+      <c r="I52" s="51"/>
+      <c r="J52" s="51"/>
+      <c r="K52" s="51"/>
+      <c r="L52" s="51"/>
       <c r="M52" s="45" t="str">
         <f aca="false">SUBSTITUTE(ROUND(M18,2),",",".")</f>
         <v>0.71</v>
@@ -7869,7 +7870,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="0" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
@@ -7885,10 +7886,10 @@
   <dimension ref="A1:W36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="0" width="7.68"/>
@@ -7975,31 +7976,31 @@
       <c r="A2" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="50" t="n">
+      <c r="B2" s="52" t="n">
         <v>0.06585</v>
       </c>
-      <c r="C2" s="50" t="n">
+      <c r="C2" s="52" t="n">
         <v>0.07017</v>
       </c>
-      <c r="D2" s="50" t="n">
+      <c r="D2" s="52" t="n">
         <v>0.07309</v>
       </c>
-      <c r="E2" s="50" t="n">
+      <c r="E2" s="52" t="n">
         <v>0.07387</v>
       </c>
-      <c r="F2" s="50" t="n">
+      <c r="F2" s="52" t="n">
         <v>0.07981</v>
       </c>
-      <c r="G2" s="50" t="n">
+      <c r="G2" s="52" t="n">
         <v>0.08658</v>
       </c>
-      <c r="H2" s="50" t="n">
+      <c r="H2" s="52" t="n">
         <v>0.08191</v>
       </c>
-      <c r="I2" s="50" t="n">
+      <c r="I2" s="52" t="n">
         <v>0.0858</v>
       </c>
-      <c r="J2" s="50" t="n">
+      <c r="J2" s="52" t="n">
         <v>0.08662</v>
       </c>
       <c r="K2" s="21" t="n">
@@ -8018,10 +8019,10 @@
       <c r="O2" s="22" t="n">
         <v>3.67881764625957</v>
       </c>
-      <c r="P2" s="50" t="n">
+      <c r="P2" s="52" t="n">
         <v>0.10765</v>
       </c>
-      <c r="Q2" s="50" t="n">
+      <c r="Q2" s="52" t="n">
         <v>0.11638</v>
       </c>
       <c r="R2" s="21" t="n">
@@ -8088,10 +8089,10 @@
       <c r="O3" s="12" t="n">
         <v>5.02285423780529</v>
       </c>
-      <c r="P3" s="49" t="n">
+      <c r="P3" s="51" t="n">
         <v>0.06946</v>
       </c>
-      <c r="Q3" s="49" t="n">
+      <c r="Q3" s="51" t="n">
         <v>0.0764</v>
       </c>
       <c r="R3" s="12" t="n">
@@ -8159,10 +8160,10 @@
       <c r="O4" s="12" t="n">
         <v>4.63208106424013</v>
       </c>
-      <c r="P4" s="49" t="n">
+      <c r="P4" s="51" t="n">
         <v>0.13771</v>
       </c>
-      <c r="Q4" s="49" t="n">
+      <c r="Q4" s="51" t="n">
         <v>0.15493</v>
       </c>
       <c r="R4" s="12" t="n">
@@ -8230,10 +8231,10 @@
       <c r="O5" s="12" t="n">
         <v>4.30711702483058</v>
       </c>
-      <c r="P5" s="49" t="n">
+      <c r="P5" s="51" t="n">
         <v>0.19644</v>
       </c>
-      <c r="Q5" s="49" t="n">
+      <c r="Q5" s="51" t="n">
         <v>0.20311</v>
       </c>
       <c r="R5" s="12" t="n">
@@ -8301,10 +8302,10 @@
       <c r="O6" s="12" t="n">
         <v>2.58348245524487</v>
       </c>
-      <c r="P6" s="49" t="n">
+      <c r="P6" s="51" t="n">
         <v>0.25492</v>
       </c>
-      <c r="Q6" s="49" t="n">
+      <c r="Q6" s="51" t="n">
         <v>0.26504</v>
       </c>
       <c r="R6" s="12" t="n">
@@ -8329,31 +8330,31 @@
       <c r="A7" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="50" t="n">
+      <c r="B7" s="52" t="n">
         <v>0.05116</v>
       </c>
-      <c r="C7" s="50" t="n">
+      <c r="C7" s="52" t="n">
         <v>0.0533</v>
       </c>
-      <c r="D7" s="50" t="n">
+      <c r="D7" s="52" t="n">
         <v>0.05468</v>
       </c>
-      <c r="E7" s="50" t="n">
+      <c r="E7" s="52" t="n">
         <v>0.05419</v>
       </c>
-      <c r="F7" s="50" t="n">
+      <c r="F7" s="52" t="n">
         <v>0.05955</v>
       </c>
-      <c r="G7" s="50" t="n">
+      <c r="G7" s="52" t="n">
         <v>0.06432</v>
       </c>
-      <c r="H7" s="50" t="n">
+      <c r="H7" s="52" t="n">
         <v>0.06115</v>
       </c>
-      <c r="I7" s="50" t="n">
+      <c r="I7" s="52" t="n">
         <v>0.06391</v>
       </c>
-      <c r="J7" s="50" t="n">
+      <c r="J7" s="52" t="n">
         <v>0.06535</v>
       </c>
       <c r="K7" s="21" t="n">
@@ -8372,10 +8373,10 @@
       <c r="O7" s="22" t="n">
         <v>3.45952969577514</v>
       </c>
-      <c r="P7" s="50" t="n">
+      <c r="P7" s="52" t="n">
         <v>0.07843</v>
       </c>
-      <c r="Q7" s="50" t="n">
+      <c r="Q7" s="52" t="n">
         <v>0.08607</v>
       </c>
       <c r="R7" s="21" t="n">
@@ -8442,10 +8443,10 @@
       <c r="O8" s="12" t="n">
         <v>4.74557215129121</v>
       </c>
-      <c r="P8" s="49" t="n">
+      <c r="P8" s="51" t="n">
         <v>0.04545</v>
       </c>
-      <c r="Q8" s="49" t="n">
+      <c r="Q8" s="51" t="n">
         <v>0.05191</v>
       </c>
       <c r="R8" s="12" t="n">
@@ -8513,10 +8514,10 @@
       <c r="O9" s="12" t="n">
         <v>4.60553266631978</v>
       </c>
-      <c r="P9" s="49" t="n">
+      <c r="P9" s="51" t="n">
         <v>0.10127</v>
       </c>
-      <c r="Q9" s="49" t="n">
+      <c r="Q9" s="51" t="n">
         <v>0.11343</v>
       </c>
       <c r="R9" s="12" t="n">
@@ -8584,10 +8585,10 @@
       <c r="O10" s="12" t="n">
         <v>4.42860584643829</v>
       </c>
-      <c r="P10" s="49" t="n">
+      <c r="P10" s="51" t="n">
         <v>0.15202</v>
       </c>
-      <c r="Q10" s="49" t="n">
+      <c r="Q10" s="51" t="n">
         <v>0.15812</v>
       </c>
       <c r="R10" s="12" t="n">
@@ -8655,10 +8656,10 @@
       <c r="O11" s="12" t="n">
         <v>2.7854430341357</v>
       </c>
-      <c r="P11" s="49" t="n">
+      <c r="P11" s="51" t="n">
         <v>0.21542</v>
       </c>
-      <c r="Q11" s="49" t="n">
+      <c r="Q11" s="51" t="n">
         <v>0.22618</v>
       </c>
       <c r="R11" s="12" t="n">
@@ -8683,31 +8684,31 @@
       <c r="A12" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="B12" s="50" t="n">
+      <c r="B12" s="52" t="n">
         <v>0.45356</v>
       </c>
-      <c r="C12" s="50" t="n">
+      <c r="C12" s="52" t="n">
         <v>0.44942</v>
       </c>
-      <c r="D12" s="50" t="n">
+      <c r="D12" s="52" t="n">
         <v>0.45464</v>
       </c>
-      <c r="E12" s="50" t="n">
+      <c r="E12" s="52" t="n">
         <v>0.45875</v>
       </c>
-      <c r="F12" s="50" t="n">
+      <c r="F12" s="52" t="n">
         <v>0.46619</v>
       </c>
-      <c r="G12" s="50" t="n">
+      <c r="G12" s="52" t="n">
         <v>0.45586</v>
       </c>
-      <c r="H12" s="50" t="n">
+      <c r="H12" s="52" t="n">
         <v>0.44215</v>
       </c>
-      <c r="I12" s="50" t="n">
+      <c r="I12" s="52" t="n">
         <v>0.44198</v>
       </c>
-      <c r="J12" s="50" t="n">
+      <c r="J12" s="52" t="n">
         <v>0.39867</v>
       </c>
       <c r="K12" s="21" t="n">
@@ -8726,10 +8727,10 @@
       <c r="O12" s="22" t="n">
         <v>-0.780315907124907</v>
       </c>
-      <c r="P12" s="50" t="n">
+      <c r="P12" s="52" t="n">
         <v>0.39901</v>
       </c>
-      <c r="Q12" s="50" t="n">
+      <c r="Q12" s="52" t="n">
         <v>0.39592</v>
       </c>
       <c r="R12" s="21" t="n">
@@ -8796,10 +8797,10 @@
       <c r="O13" s="12" t="n">
         <v>-0.552645879379055</v>
       </c>
-      <c r="P13" s="49" t="n">
+      <c r="P13" s="51" t="n">
         <v>0.34336</v>
       </c>
-      <c r="Q13" s="49" t="n">
+      <c r="Q13" s="51" t="n">
         <v>0.33026</v>
       </c>
       <c r="R13" s="12" t="n">
@@ -8867,10 +8868,10 @@
       <c r="O14" s="12" t="n">
         <v>1.68126902842132</v>
       </c>
-      <c r="P14" s="49" t="n">
+      <c r="P14" s="51" t="n">
         <v>0.44325</v>
       </c>
-      <c r="Q14" s="49" t="n">
+      <c r="Q14" s="51" t="n">
         <v>0.47302</v>
       </c>
       <c r="R14" s="12" t="n">
@@ -8938,10 +8939,10 @@
       <c r="O15" s="12" t="n">
         <v>1.72244999471303</v>
       </c>
-      <c r="P15" s="49" t="n">
+      <c r="P15" s="51" t="n">
         <v>0.53431</v>
       </c>
-      <c r="Q15" s="49" t="n">
+      <c r="Q15" s="51" t="n">
         <v>0.53862</v>
       </c>
       <c r="R15" s="12" t="n">
@@ -8966,31 +8967,31 @@
       <c r="A16" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="51" t="n">
+      <c r="B16" s="53" t="n">
         <v>0.61815</v>
       </c>
-      <c r="C16" s="51" t="n">
+      <c r="C16" s="53" t="n">
         <v>0.64535</v>
       </c>
-      <c r="D16" s="51" t="n">
+      <c r="D16" s="53" t="n">
         <v>0.65481</v>
       </c>
-      <c r="E16" s="51" t="n">
+      <c r="E16" s="53" t="n">
         <v>0.66586</v>
       </c>
-      <c r="F16" s="51" t="n">
+      <c r="F16" s="53" t="n">
         <v>0.65903</v>
       </c>
-      <c r="G16" s="51" t="n">
+      <c r="G16" s="53" t="n">
         <v>0.67066</v>
       </c>
-      <c r="H16" s="51" t="n">
+      <c r="H16" s="53" t="n">
         <v>0.64553</v>
       </c>
-      <c r="I16" s="51" t="n">
+      <c r="I16" s="53" t="n">
         <v>0.64396</v>
       </c>
-      <c r="J16" s="51" t="n">
+      <c r="J16" s="53" t="n">
         <v>0.60934</v>
       </c>
       <c r="K16" s="28" t="n">
@@ -9009,10 +9010,10 @@
       <c r="O16" s="28" t="n">
         <v>1.14675304970047</v>
       </c>
-      <c r="P16" s="52" t="n">
+      <c r="P16" s="54" t="n">
         <v>0.60519</v>
       </c>
-      <c r="Q16" s="52" t="n">
+      <c r="Q16" s="54" t="n">
         <v>0.61365</v>
       </c>
       <c r="R16" s="28" t="n">
@@ -9431,7 +9432,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="0" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
@@ -9447,10 +9448,10 @@
   <dimension ref="A1:W16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="0" width="7.68"/>
@@ -9537,47 +9538,47 @@
       <c r="A2" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="53" t="n">
+      <c r="B2" s="55" t="n">
         <v>7.75540699960676</v>
       </c>
-      <c r="C2" s="53" t="n">
+      <c r="C2" s="55" t="n">
         <v>7.92289114043355</v>
       </c>
-      <c r="D2" s="53" t="n">
+      <c r="D2" s="55" t="n">
         <v>8.07077898456582</v>
       </c>
-      <c r="E2" s="53" t="n">
+      <c r="E2" s="55" t="n">
         <v>8.17140073831009</v>
       </c>
-      <c r="F2" s="53" t="n">
+      <c r="F2" s="55" t="n">
         <v>8.07135317711632</v>
       </c>
-      <c r="G2" s="53" t="n">
+      <c r="G2" s="55" t="n">
         <v>8.29358568887132</v>
       </c>
-      <c r="H2" s="53" t="n">
+      <c r="H2" s="55" t="n">
         <v>8.15120918090923</v>
       </c>
-      <c r="I2" s="53" t="n">
+      <c r="I2" s="55" t="n">
         <v>8.18288461538462</v>
       </c>
-      <c r="J2" s="53" t="n">
+      <c r="J2" s="55" t="n">
         <v>7.96708255906557</v>
       </c>
-      <c r="K2" s="53" t="n">
+      <c r="K2" s="55" t="n">
         <v>2.72939330546468</v>
       </c>
       <c r="L2" s="9" t="str">
         <f aca="false">_xlfn.CONCAT(M12," [",N12," ; ",O12,"]")</f>
         <v>0.4 [-8.16 ; 9.75]</v>
       </c>
-      <c r="M2" s="53" t="n">
+      <c r="M2" s="55" t="n">
         <v>0.39543296188711</v>
       </c>
-      <c r="N2" s="53" t="n">
+      <c r="N2" s="55" t="n">
         <v>-8.16289829882444</v>
       </c>
-      <c r="O2" s="53" t="n">
+      <c r="O2" s="55" t="n">
         <v>9.75131807187408</v>
       </c>
       <c r="P2" s="12" t="n">
@@ -9607,47 +9608,47 @@
       <c r="A3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="53" t="n">
+      <c r="B3" s="55" t="n">
         <v>7.67341772151899</v>
       </c>
-      <c r="C3" s="53" t="n">
+      <c r="C3" s="55" t="n">
         <v>7.66206896551724</v>
       </c>
-      <c r="D3" s="53" t="n">
+      <c r="D3" s="55" t="n">
         <v>7.86795491143317</v>
       </c>
-      <c r="E3" s="53" t="n">
+      <c r="E3" s="55" t="n">
         <v>7.80508229858504</v>
       </c>
-      <c r="F3" s="53" t="n">
+      <c r="F3" s="55" t="n">
         <v>8.23288508557457</v>
       </c>
-      <c r="G3" s="53" t="n">
+      <c r="G3" s="55" t="n">
         <v>8.08261662757363</v>
       </c>
-      <c r="H3" s="53" t="n">
+      <c r="H3" s="55" t="n">
         <v>7.83238209672574</v>
       </c>
-      <c r="I3" s="53" t="n">
+      <c r="I3" s="55" t="n">
         <v>8.21682398667407</v>
       </c>
-      <c r="J3" s="53" t="n">
+      <c r="J3" s="55" t="n">
         <v>7.88510101010101</v>
       </c>
-      <c r="K3" s="53" t="n">
+      <c r="K3" s="55" t="n">
         <v>2.7586571755163</v>
       </c>
       <c r="L3" s="17" t="str">
         <f aca="false">_xlfn.CONCAT(M13," [",N13," ; ",O13,"]")</f>
         <v>0.57 [-8.08 ; 10.04]</v>
       </c>
-      <c r="M3" s="53" t="n">
+      <c r="M3" s="55" t="n">
         <v>0.573679413776196</v>
       </c>
-      <c r="N3" s="53" t="n">
+      <c r="N3" s="55" t="n">
         <v>-8.07615170822612</v>
       </c>
-      <c r="O3" s="53" t="n">
+      <c r="O3" s="55" t="n">
         <v>10.0374405422952</v>
       </c>
       <c r="P3" s="12" t="n">
@@ -9678,47 +9679,47 @@
       <c r="A4" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="53" t="n">
+      <c r="B4" s="55" t="n">
         <v>8.24208475401851</v>
       </c>
-      <c r="C4" s="53" t="n">
+      <c r="C4" s="55" t="n">
         <v>8.26049329294678</v>
       </c>
-      <c r="D4" s="53" t="n">
+      <c r="D4" s="55" t="n">
         <v>8.44591029023747</v>
       </c>
-      <c r="E4" s="53" t="n">
+      <c r="E4" s="55" t="n">
         <v>8.30840759395583</v>
       </c>
-      <c r="F4" s="53" t="n">
+      <c r="F4" s="55" t="n">
         <v>8.51545064377682</v>
       </c>
-      <c r="G4" s="53" t="n">
+      <c r="G4" s="55" t="n">
         <v>8.51653764954258</v>
       </c>
-      <c r="H4" s="53" t="n">
+      <c r="H4" s="55" t="n">
         <v>8.51809145129225</v>
       </c>
-      <c r="I4" s="53" t="n">
+      <c r="I4" s="55" t="n">
         <v>8.60208695652174</v>
       </c>
-      <c r="J4" s="53" t="n">
+      <c r="J4" s="55" t="n">
         <v>8.01519861830743</v>
       </c>
-      <c r="K4" s="53" t="n">
+      <c r="K4" s="55" t="n">
         <v>-2.75277605705842</v>
       </c>
       <c r="L4" s="17" t="str">
         <f aca="false">_xlfn.CONCAT(M14," [",N14," ; ",O14,"]")</f>
         <v>0.09 [-8.28 ; 9.24]</v>
       </c>
-      <c r="M4" s="53" t="n">
+      <c r="M4" s="55" t="n">
         <v>0.0934610795480628</v>
       </c>
-      <c r="N4" s="53" t="n">
+      <c r="N4" s="55" t="n">
         <v>-8.28381900099938</v>
       </c>
-      <c r="O4" s="53" t="n">
+      <c r="O4" s="55" t="n">
         <v>9.23591499074925</v>
       </c>
       <c r="P4" s="12" t="n">
@@ -9749,47 +9750,47 @@
       <c r="A5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="53" t="n">
+      <c r="B5" s="55" t="n">
         <v>8.05954088952654</v>
       </c>
-      <c r="C5" s="53" t="n">
+      <c r="C5" s="55" t="n">
         <v>8.25426509186352</v>
       </c>
-      <c r="D5" s="53" t="n">
+      <c r="D5" s="55" t="n">
         <v>8.43311181739382</v>
       </c>
-      <c r="E5" s="53" t="n">
+      <c r="E5" s="55" t="n">
         <v>8.57896229089878</v>
       </c>
-      <c r="F5" s="53" t="n">
+      <c r="F5" s="55" t="n">
         <v>8.12945537496436</v>
       </c>
-      <c r="G5" s="53" t="n">
+      <c r="G5" s="55" t="n">
         <v>8.51593677118425</v>
       </c>
-      <c r="H5" s="53" t="n">
+      <c r="H5" s="55" t="n">
         <v>8.43861410996736</v>
       </c>
-      <c r="I5" s="53" t="n">
+      <c r="I5" s="55" t="n">
         <v>8.74262607040913</v>
       </c>
-      <c r="J5" s="53" t="n">
+      <c r="J5" s="55" t="n">
         <v>8.322454308094</v>
       </c>
-      <c r="K5" s="53" t="n">
+      <c r="K5" s="55" t="n">
         <v>3.26213890060552</v>
       </c>
       <c r="L5" s="17" t="str">
         <f aca="false">_xlfn.CONCAT(M15," [",N15," ; ",O15,"]")</f>
         <v>0.49 [-7.92 ; 9.67]</v>
       </c>
-      <c r="M5" s="53" t="n">
+      <c r="M5" s="55" t="n">
         <v>0.491058851135362</v>
       </c>
-      <c r="N5" s="53" t="n">
+      <c r="N5" s="55" t="n">
         <v>-7.91717539441853</v>
       </c>
-      <c r="O5" s="53" t="n">
+      <c r="O5" s="55" t="n">
         <v>9.66706280217915</v>
       </c>
       <c r="P5" s="12" t="n">
@@ -9820,47 +9821,47 @@
       <c r="A6" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="54" t="n">
+      <c r="B6" s="56" t="n">
         <v>7.53658536585366</v>
       </c>
-      <c r="C6" s="54" t="n">
+      <c r="C6" s="56" t="n">
         <v>7.81442792183852</v>
       </c>
-      <c r="D6" s="54" t="n">
+      <c r="D6" s="56" t="n">
         <v>7.91194299691588</v>
       </c>
-      <c r="E6" s="54" t="n">
+      <c r="E6" s="56" t="n">
         <v>8.11879593274942</v>
       </c>
-      <c r="F6" s="54" t="n">
+      <c r="F6" s="56" t="n">
         <v>7.89175729240777</v>
       </c>
-      <c r="G6" s="54" t="n">
+      <c r="G6" s="56" t="n">
         <v>8.22324190554754</v>
       </c>
-      <c r="H6" s="54" t="n">
+      <c r="H6" s="56" t="n">
         <v>8.05517373043146</v>
       </c>
-      <c r="I6" s="54" t="n">
+      <c r="I6" s="56" t="n">
         <v>7.81915209012748</v>
       </c>
-      <c r="J6" s="54" t="n">
+      <c r="J6" s="56" t="n">
         <v>7.83723432875975</v>
       </c>
-      <c r="K6" s="54" t="n">
+      <c r="K6" s="56" t="n">
         <v>3.98919335894818</v>
       </c>
       <c r="L6" s="29" t="str">
         <f aca="false">_xlfn.CONCAT(M16," [",N16," ; ",O16,"]")</f>
         <v>0.34 [-8.29 ; 9.78]</v>
       </c>
-      <c r="M6" s="54" t="n">
+      <c r="M6" s="56" t="n">
         <v>0.339235624689071</v>
       </c>
-      <c r="N6" s="54" t="n">
+      <c r="N6" s="56" t="n">
         <v>-8.29296895804491</v>
       </c>
-      <c r="O6" s="54" t="n">
+      <c r="O6" s="56" t="n">
         <v>9.78397284654082</v>
       </c>
       <c r="P6" s="28" t="n">
@@ -10025,7 +10026,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="0" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
@@ -10040,7 +10041,7 @@
   </sheetPr>
   <dimension ref="A2:Q407"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="R17" activeCellId="0" sqref="R17"/>
     </sheetView>
   </sheetViews>
@@ -10048,94 +10049,91 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="52.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="55" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="49.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="55" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="5.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="52.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="55" width="4.17"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="13" style="55" width="11.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="55" width="12.83"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="17" min="15" style="55" width="11.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="55" width="19.45"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="19" style="55" width="11.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="4.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="19.45"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="56" t="n">
+      <c r="A2" s="57" t="n">
         <v>2011</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="57" t="s">
+      <c r="B2" s="57"/>
+      <c r="C2" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="D2" s="58"/>
-      <c r="E2" s="56" t="n">
+      <c r="D2" s="59"/>
+      <c r="E2" s="57" t="n">
         <v>2019</v>
       </c>
-      <c r="F2" s="56"/>
-      <c r="G2" s="57" t="s">
+      <c r="F2" s="57"/>
+      <c r="G2" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="H2" s="58"/>
-      <c r="I2" s="56" t="n">
+      <c r="H2" s="59"/>
+      <c r="I2" s="57" t="n">
         <v>2021</v>
       </c>
-      <c r="J2" s="56"/>
-      <c r="K2" s="57" t="s">
+      <c r="J2" s="57"/>
+      <c r="K2" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="M2" s="59" t="s">
+      <c r="M2" s="60" t="s">
         <v>78</v>
       </c>
-      <c r="N2" s="59" t="s">
+      <c r="N2" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="O2" s="59" t="s">
+      <c r="O2" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="P2" s="59" t="s">
+      <c r="P2" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="Q2" s="59" t="s">
+      <c r="Q2" s="60" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="61" t="s">
         <v>83</v>
       </c>
-      <c r="B3" s="60" t="str">
+      <c r="B3" s="61" t="str">
         <f aca="false">VLOOKUP(A3,CIDS_description!$A$1:$D$61,4,0)</f>
         <v>Pneumonia, unspecified organisms</v>
       </c>
-      <c r="C3" s="61" t="n">
+      <c r="C3" s="62" t="n">
         <v>0.406843403035683</v>
       </c>
-      <c r="D3" s="58"/>
-      <c r="E3" s="60" t="s">
+      <c r="D3" s="59"/>
+      <c r="E3" s="61" t="s">
         <v>83</v>
       </c>
-      <c r="F3" s="60" t="str">
+      <c r="F3" s="61" t="str">
         <f aca="false">VLOOKUP(E3,CIDS_description!$A$1:$D$61,4,0)</f>
         <v>Pneumonia, unspecified organisms</v>
       </c>
-      <c r="G3" s="61" t="n">
+      <c r="G3" s="62" t="n">
         <v>0.426888693433939</v>
       </c>
-      <c r="H3" s="58"/>
-      <c r="I3" s="60" t="s">
+      <c r="H3" s="59"/>
+      <c r="I3" s="61" t="s">
         <v>83</v>
       </c>
-      <c r="J3" s="60" t="str">
+      <c r="J3" s="61" t="str">
         <f aca="false">VLOOKUP(I3,CIDS_description!$A$1:$D$61,4,0)</f>
         <v>Pneumonia, unspecified organisms</v>
       </c>
-      <c r="K3" s="61" t="n">
+      <c r="K3" s="62" t="n">
         <v>0.424412913654528</v>
       </c>
-      <c r="M3" s="62" t="n">
+      <c r="M3" s="58" t="n">
         <v>1</v>
       </c>
       <c r="N3" s="63" t="n">
@@ -10162,7 +10160,7 @@
       <c r="C4" s="67" t="n">
         <v>0.124127800220345</v>
       </c>
-      <c r="D4" s="58"/>
+      <c r="D4" s="59"/>
       <c r="E4" s="66" t="s">
         <v>85</v>
       </c>
@@ -10173,7 +10171,7 @@
       <c r="G4" s="67" t="n">
         <v>0.175134548107842</v>
       </c>
-      <c r="H4" s="58"/>
+      <c r="H4" s="59"/>
       <c r="I4" s="66" t="s">
         <v>85</v>
       </c>
@@ -10202,36 +10200,36 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="61" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="60" t="str">
+      <c r="B5" s="61" t="str">
         <f aca="false">VLOOKUP(A5,CIDS_description!$A$1:$D$61,4,0)</f>
         <v>Other pneumonia, unspecified organism</v>
       </c>
-      <c r="C5" s="61" t="n">
+      <c r="C5" s="62" t="n">
         <v>0.111470376271196</v>
       </c>
-      <c r="D5" s="58"/>
-      <c r="E5" s="60" t="s">
+      <c r="D5" s="59"/>
+      <c r="E5" s="61" t="s">
         <v>84</v>
       </c>
-      <c r="F5" s="60" t="str">
+      <c r="F5" s="61" t="str">
         <f aca="false">VLOOKUP(E5,CIDS_description!$A$1:$D$61,4,0)</f>
         <v>Bronchopneumonia, unspecified organism</v>
       </c>
-      <c r="G5" s="61" t="n">
+      <c r="G5" s="62" t="n">
         <v>0.12760222969476</v>
       </c>
-      <c r="H5" s="58"/>
-      <c r="I5" s="60" t="s">
+      <c r="H5" s="59"/>
+      <c r="I5" s="61" t="s">
         <v>84</v>
       </c>
-      <c r="J5" s="60" t="str">
+      <c r="J5" s="61" t="str">
         <f aca="false">VLOOKUP(I5,CIDS_description!$A$1:$D$61,4,0)</f>
         <v>Bronchopneumonia, unspecified organism</v>
       </c>
-      <c r="K5" s="61" t="n">
+      <c r="K5" s="62" t="n">
         <v>0.112675676889228</v>
       </c>
       <c r="M5" s="68" t="n">
@@ -10262,7 +10260,7 @@
       <c r="C6" s="67" t="n">
         <v>0.0897948138800913</v>
       </c>
-      <c r="D6" s="58"/>
+      <c r="D6" s="59"/>
       <c r="E6" s="66" t="s">
         <v>87</v>
       </c>
@@ -10273,7 +10271,7 @@
       <c r="G6" s="67" t="n">
         <v>0.0829234906997067</v>
       </c>
-      <c r="H6" s="58"/>
+      <c r="H6" s="59"/>
       <c r="I6" s="66" t="s">
         <v>87</v>
       </c>
@@ -10302,36 +10300,36 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="60" t="s">
+      <c r="A7" s="61" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="60" t="str">
+      <c r="B7" s="61" t="str">
         <f aca="false">VLOOKUP(A7,CIDS_description!$A$1:$D$61,4,0)</f>
         <v>Unspecified bacterial pneumonia</v>
       </c>
-      <c r="C7" s="61" t="n">
+      <c r="C7" s="62" t="n">
         <v>0.0649604179379775</v>
       </c>
-      <c r="D7" s="58"/>
-      <c r="E7" s="60" t="s">
+      <c r="D7" s="59"/>
+      <c r="E7" s="61" t="s">
         <v>86</v>
       </c>
-      <c r="F7" s="60" t="str">
+      <c r="F7" s="61" t="str">
         <f aca="false">VLOOKUP(E7,CIDS_description!$A$1:$D$61,4,0)</f>
         <v>Other pneumonia, unspecified organism</v>
       </c>
-      <c r="G7" s="61" t="n">
+      <c r="G7" s="62" t="n">
         <v>0.0612345902469237</v>
       </c>
-      <c r="H7" s="58"/>
-      <c r="I7" s="60" t="s">
+      <c r="H7" s="59"/>
+      <c r="I7" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="J7" s="60" t="str">
+      <c r="J7" s="61" t="str">
         <f aca="false">VLOOKUP(I7,CIDS_description!$A$1:$D$61,4,0)</f>
         <v>Viral pneumonia, unspecified</v>
       </c>
-      <c r="K7" s="61" t="n">
+      <c r="K7" s="62" t="n">
         <v>0.0495397602263033</v>
       </c>
       <c r="M7" s="68" t="n">
@@ -10362,7 +10360,7 @@
       <c r="C8" s="67" t="n">
         <v>0.0626492783556394</v>
       </c>
-      <c r="D8" s="58"/>
+      <c r="D8" s="59"/>
       <c r="E8" s="66" t="s">
         <v>89</v>
       </c>
@@ -10373,7 +10371,7 @@
       <c r="G8" s="67" t="n">
         <v>0.0300827792562593</v>
       </c>
-      <c r="H8" s="58"/>
+      <c r="H8" s="59"/>
       <c r="I8" s="66" t="s">
         <v>86</v>
       </c>
@@ -10402,36 +10400,36 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="60" t="s">
+      <c r="A9" s="61" t="s">
         <v>90</v>
       </c>
-      <c r="B9" s="60" t="str">
+      <c r="B9" s="61" t="str">
         <f aca="false">VLOOKUP(A9,CIDS_description!$A$1:$D$61,4,0)</f>
         <v>Pneumonia due to other specified infectious organisms</v>
       </c>
-      <c r="C9" s="61" t="n">
+      <c r="C9" s="62" t="n">
         <v>0.0446212851261463</v>
       </c>
-      <c r="D9" s="58"/>
-      <c r="E9" s="60" t="s">
+      <c r="D9" s="59"/>
+      <c r="E9" s="61" t="s">
         <v>90</v>
       </c>
-      <c r="F9" s="60" t="str">
+      <c r="F9" s="61" t="str">
         <f aca="false">VLOOKUP(E9,CIDS_description!$A$1:$D$61,4,0)</f>
         <v>Pneumonia due to other specified infectious organisms</v>
       </c>
-      <c r="G9" s="61" t="n">
+      <c r="G9" s="62" t="n">
         <v>0.0207499625273268</v>
       </c>
-      <c r="H9" s="58"/>
-      <c r="I9" s="60" t="s">
+      <c r="H9" s="59"/>
+      <c r="I9" s="61" t="s">
         <v>89</v>
       </c>
-      <c r="J9" s="60" t="str">
+      <c r="J9" s="61" t="str">
         <f aca="false">VLOOKUP(I9,CIDS_description!$A$1:$D$61,4,0)</f>
         <v>Other viral pneumonia</v>
       </c>
-      <c r="K9" s="61" t="n">
+      <c r="K9" s="62" t="n">
         <v>0.037178393426429</v>
       </c>
       <c r="M9" s="68" t="n">
@@ -10462,7 +10460,7 @@
       <c r="C10" s="67" t="n">
         <v>0.0234537868726167</v>
       </c>
-      <c r="D10" s="58"/>
+      <c r="D10" s="59"/>
       <c r="E10" s="66" t="s">
         <v>91</v>
       </c>
@@ -10473,7 +10471,7 @@
       <c r="G10" s="67" t="n">
         <v>0.0200203059467011</v>
       </c>
-      <c r="H10" s="58"/>
+      <c r="H10" s="59"/>
       <c r="I10" s="66" t="s">
         <v>91</v>
       </c>
@@ -10502,36 +10500,36 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="60" t="s">
+      <c r="A11" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="B11" s="60" t="str">
+      <c r="B11" s="61" t="str">
         <f aca="false">VLOOKUP(A11,CIDS_description!$A$1:$D$61,4,0)</f>
         <v>Lobar pneumonia, unspecified organism</v>
       </c>
-      <c r="C11" s="61" t="n">
+      <c r="C11" s="62" t="n">
         <v>0.0184974003131221</v>
       </c>
-      <c r="D11" s="58"/>
-      <c r="E11" s="60" t="s">
+      <c r="D11" s="59"/>
+      <c r="E11" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="F11" s="60" t="str">
+      <c r="F11" s="61" t="str">
         <f aca="false">VLOOKUP(E11,CIDS_description!$A$1:$D$61,4,0)</f>
         <v>Viral pneumonia, unspecified</v>
       </c>
-      <c r="G11" s="61" t="n">
+      <c r="G11" s="62" t="n">
         <v>0.0162334448557797</v>
       </c>
-      <c r="H11" s="58"/>
-      <c r="I11" s="60" t="s">
+      <c r="H11" s="59"/>
+      <c r="I11" s="61" t="s">
         <v>90</v>
       </c>
-      <c r="J11" s="60" t="str">
+      <c r="J11" s="61" t="str">
         <f aca="false">VLOOKUP(I11,CIDS_description!$A$1:$D$61,4,0)</f>
         <v>Pneumonia due to other specified infectious organisms</v>
       </c>
-      <c r="K11" s="61" t="n">
+      <c r="K11" s="62" t="n">
         <v>0.0152485294777962</v>
       </c>
       <c r="M11" s="68" t="n">
@@ -10562,7 +10560,7 @@
       <c r="C12" s="67" t="n">
         <v>0.0157886453187688</v>
       </c>
-      <c r="D12" s="58"/>
+      <c r="D12" s="59"/>
       <c r="E12" s="66" t="s">
         <v>92</v>
       </c>
@@ -10573,7 +10571,7 @@
       <c r="G12" s="67" t="n">
         <v>0.0073955502261087</v>
       </c>
-      <c r="H12" s="58"/>
+      <c r="H12" s="59"/>
       <c r="I12" s="66" t="s">
         <v>93</v>
       </c>
@@ -17719,7 +17717,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="0" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
@@ -17739,7 +17737,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="2.54"/>
@@ -18614,4 +18612,2787 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:Y76"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L33" activeCellId="0" sqref="L33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="2" style="0" width="10.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.8"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="15" min="13" style="0" width="10.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="21.86"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="22" min="20" style="0" width="11.54"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="37" t="n">
+        <v>2011</v>
+      </c>
+      <c r="C1" s="37" t="n">
+        <v>2012</v>
+      </c>
+      <c r="D1" s="37" t="n">
+        <v>2013</v>
+      </c>
+      <c r="E1" s="37" t="n">
+        <v>2014</v>
+      </c>
+      <c r="F1" s="37" t="n">
+        <v>2015</v>
+      </c>
+      <c r="G1" s="37" t="n">
+        <v>2016</v>
+      </c>
+      <c r="H1" s="37" t="n">
+        <v>2017</v>
+      </c>
+      <c r="I1" s="37" t="n">
+        <v>2018</v>
+      </c>
+      <c r="J1" s="37" t="n">
+        <v>2019</v>
+      </c>
+      <c r="K1" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="O1" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1" s="37" t="n">
+        <v>2020</v>
+      </c>
+      <c r="Q1" s="37" t="n">
+        <v>2021</v>
+      </c>
+      <c r="R1" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="S1" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="T1" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="U1" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="V1" s="39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" s="41" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="20" t="n">
+        <v>5285633</v>
+      </c>
+      <c r="C2" s="20" t="n">
+        <v>5213074</v>
+      </c>
+      <c r="D2" s="20" t="n">
+        <v>5246687</v>
+      </c>
+      <c r="E2" s="20" t="n">
+        <v>5304161</v>
+      </c>
+      <c r="F2" s="20" t="n">
+        <v>5265162</v>
+      </c>
+      <c r="G2" s="20" t="n">
+        <v>5218627</v>
+      </c>
+      <c r="H2" s="20" t="n">
+        <v>5286445</v>
+      </c>
+      <c r="I2" s="20" t="n">
+        <v>5445551</v>
+      </c>
+      <c r="J2" s="20" t="n">
+        <v>5622312</v>
+      </c>
+      <c r="K2" s="21" t="n">
+        <v>6.36970065836959</v>
+      </c>
+      <c r="L2" s="9" t="str">
+        <f aca="false">_xlfn.CONCAT(M36," [",N36," ; ",O36,"]")</f>
+        <v>0.64 [0.63 ; 0.65]</v>
+      </c>
+      <c r="M2" s="21" t="n">
+        <v>0.640487531477563</v>
+      </c>
+      <c r="N2" s="21" t="n">
+        <v>0.629447580451981</v>
+      </c>
+      <c r="O2" s="21" t="n">
+        <v>0.651528693684589</v>
+      </c>
+      <c r="P2" s="20" t="n">
+        <v>4858330</v>
+      </c>
+      <c r="Q2" s="20" t="n">
+        <v>5353034</v>
+      </c>
+      <c r="R2" s="21" t="n">
+        <v>-4.7894531644633</v>
+      </c>
+      <c r="S2" s="13" t="str">
+        <f aca="false">_xlfn.CONCAT(T36," [",U36," ; ",V36,"]")</f>
+        <v>-2.52 [-2.58 ; -2.46]</v>
+      </c>
+      <c r="T2" s="12" t="n">
+        <v>-2.51900622250806</v>
+      </c>
+      <c r="U2" s="12" t="n">
+        <v>-2.57780420799607</v>
+      </c>
+      <c r="V2" s="12" t="n">
+        <v>-2.46017275020856</v>
+      </c>
+    </row>
+    <row r="3" s="41" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="11" t="n">
+        <v>327734</v>
+      </c>
+      <c r="C3" s="11" t="n">
+        <v>339743</v>
+      </c>
+      <c r="D3" s="11" t="n">
+        <v>350228</v>
+      </c>
+      <c r="E3" s="11" t="n">
+        <v>367284</v>
+      </c>
+      <c r="F3" s="11" t="n">
+        <v>372322</v>
+      </c>
+      <c r="G3" s="11" t="n">
+        <v>378607</v>
+      </c>
+      <c r="H3" s="11" t="n">
+        <v>395949</v>
+      </c>
+      <c r="I3" s="11" t="n">
+        <v>413039</v>
+      </c>
+      <c r="J3" s="11" t="n">
+        <v>443166</v>
+      </c>
+      <c r="K3" s="12" t="n">
+        <v>35.2212464986849</v>
+      </c>
+      <c r="L3" s="17" t="str">
+        <f aca="false">_xlfn.CONCAT(M37," [",N37," ; ",O37,"]")</f>
+        <v>3.54 [3.5 ; 3.58]</v>
+      </c>
+      <c r="M3" s="12" t="n">
+        <v>3.53963074673582</v>
+      </c>
+      <c r="N3" s="12" t="n">
+        <v>3.49683407957595</v>
+      </c>
+      <c r="O3" s="12" t="n">
+        <v>3.58244511061789</v>
+      </c>
+      <c r="P3" s="11" t="n">
+        <v>529750</v>
+      </c>
+      <c r="Q3" s="11" t="n">
+        <v>693891</v>
+      </c>
+      <c r="R3" s="12" t="n">
+        <v>56.5758654770447</v>
+      </c>
+      <c r="S3" s="18" t="str">
+        <f aca="false">_xlfn.CONCAT(T37," [",U37," ; ",V37,"]")</f>
+        <v>25.56 [25.32 ; 25.79]</v>
+      </c>
+      <c r="T3" s="12" t="n">
+        <v>25.5552992897818</v>
+      </c>
+      <c r="U3" s="12" t="n">
+        <v>25.3190512496173</v>
+      </c>
+      <c r="V3" s="12" t="n">
+        <v>25.7919926982755</v>
+      </c>
+    </row>
+    <row r="4" s="41" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="11" t="n">
+        <v>4957899</v>
+      </c>
+      <c r="C4" s="11" t="n">
+        <v>4873331</v>
+      </c>
+      <c r="D4" s="11" t="n">
+        <v>4896459</v>
+      </c>
+      <c r="E4" s="11" t="n">
+        <v>4936877</v>
+      </c>
+      <c r="F4" s="11" t="n">
+        <v>4892840</v>
+      </c>
+      <c r="G4" s="11" t="n">
+        <v>4840020</v>
+      </c>
+      <c r="H4" s="11" t="n">
+        <v>4890496</v>
+      </c>
+      <c r="I4" s="11" t="n">
+        <v>5032512</v>
+      </c>
+      <c r="J4" s="11" t="n">
+        <v>5179146</v>
+      </c>
+      <c r="K4" s="12" t="n">
+        <v>4.4625152710856</v>
+      </c>
+      <c r="L4" s="17" t="str">
+        <f aca="false">_xlfn.CONCAT(M38," [",N38," ; ",O38,"]")</f>
+        <v>0.42 [0.41 ; 0.43]</v>
+      </c>
+      <c r="M4" s="12" t="n">
+        <v>0.423520313316983</v>
+      </c>
+      <c r="N4" s="12" t="n">
+        <v>0.412093045741768</v>
+      </c>
+      <c r="O4" s="12" t="n">
+        <v>0.434948881357533</v>
+      </c>
+      <c r="P4" s="11" t="n">
+        <v>4328580</v>
+      </c>
+      <c r="Q4" s="11" t="n">
+        <v>4659143</v>
+      </c>
+      <c r="R4" s="12" t="n">
+        <v>-10.0403232502038</v>
+      </c>
+      <c r="S4" s="18" t="str">
+        <f aca="false">_xlfn.CONCAT(T38," [",U38," ; ",V38,"]")</f>
+        <v>-5.36 [-5.42 ; -5.3]</v>
+      </c>
+      <c r="T4" s="12" t="n">
+        <v>-5.35964320029102</v>
+      </c>
+      <c r="U4" s="12" t="n">
+        <v>-5.42002748407797</v>
+      </c>
+      <c r="V4" s="12" t="n">
+        <v>-5.2992203643494</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="11" t="n">
+        <v>2257441</v>
+      </c>
+      <c r="C5" s="11" t="n">
+        <v>2208659</v>
+      </c>
+      <c r="D5" s="11" t="n">
+        <v>2168720</v>
+      </c>
+      <c r="E5" s="11" t="n">
+        <v>2177013</v>
+      </c>
+      <c r="F5" s="11" t="n">
+        <v>2107769</v>
+      </c>
+      <c r="G5" s="11" t="n">
+        <v>2063703</v>
+      </c>
+      <c r="H5" s="11" t="n">
+        <v>2038668</v>
+      </c>
+      <c r="I5" s="11" t="n">
+        <v>2097178</v>
+      </c>
+      <c r="J5" s="11" t="n">
+        <v>2137618</v>
+      </c>
+      <c r="K5" s="12" t="n">
+        <v>-5.30791280923843</v>
+      </c>
+      <c r="L5" s="17" t="str">
+        <f aca="false">_xlfn.CONCAT(M39," [",N39," ; ",O39,"]")</f>
+        <v>-0.92 [-0.94 ; -0.9]</v>
+      </c>
+      <c r="M5" s="12" t="n">
+        <v>-0.920570653664787</v>
+      </c>
+      <c r="N5" s="12" t="n">
+        <v>-0.937711176959255</v>
+      </c>
+      <c r="O5" s="12" t="n">
+        <v>-0.903427164584436</v>
+      </c>
+      <c r="P5" s="11" t="n">
+        <v>1797093</v>
+      </c>
+      <c r="Q5" s="11" t="n">
+        <v>1973898</v>
+      </c>
+      <c r="R5" s="12" t="n">
+        <v>-7.65899239246676</v>
+      </c>
+      <c r="S5" s="18" t="str">
+        <f aca="false">_xlfn.CONCAT(T39," [",U39," ; ",V39,"]")</f>
+        <v>-4.07 [-4.17 ; -3.98]</v>
+      </c>
+      <c r="T5" s="12" t="n">
+        <v>-4.07226653745715</v>
+      </c>
+      <c r="U5" s="12" t="n">
+        <v>-4.16699236216439</v>
+      </c>
+      <c r="V5" s="12" t="n">
+        <v>-3.97744708131657</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="11" t="n">
+        <v>83687</v>
+      </c>
+      <c r="C6" s="11" t="n">
+        <v>84820</v>
+      </c>
+      <c r="D6" s="11" t="n">
+        <v>83926</v>
+      </c>
+      <c r="E6" s="11" t="n">
+        <v>85694</v>
+      </c>
+      <c r="F6" s="11" t="n">
+        <v>84740</v>
+      </c>
+      <c r="G6" s="11" t="n">
+        <v>85256</v>
+      </c>
+      <c r="H6" s="11" t="n">
+        <v>86869</v>
+      </c>
+      <c r="I6" s="11" t="n">
+        <v>88797</v>
+      </c>
+      <c r="J6" s="11" t="n">
+        <v>95226</v>
+      </c>
+      <c r="K6" s="12" t="n">
+        <v>13.7882825289471</v>
+      </c>
+      <c r="L6" s="17" t="str">
+        <f aca="false">_xlfn.CONCAT(M40," [",N40," ; ",O40,"]")</f>
+        <v>1.23 [1.14 ; 1.32]</v>
+      </c>
+      <c r="M6" s="12" t="n">
+        <v>1.23113901641465</v>
+      </c>
+      <c r="N6" s="12" t="n">
+        <v>1.14408648459332</v>
+      </c>
+      <c r="O6" s="12" t="n">
+        <v>1.31826647247086</v>
+      </c>
+      <c r="P6" s="11" t="n">
+        <v>109852</v>
+      </c>
+      <c r="Q6" s="11" t="n">
+        <v>168900</v>
+      </c>
+      <c r="R6" s="12" t="n">
+        <v>77.3675256757608</v>
+      </c>
+      <c r="S6" s="18" t="str">
+        <f aca="false">_xlfn.CONCAT(T40," [",U40," ; ",V40,"]")</f>
+        <v>34.97 [34.43 ; 35.52]</v>
+      </c>
+      <c r="T6" s="12" t="n">
+        <v>34.9739318671415</v>
+      </c>
+      <c r="U6" s="12" t="n">
+        <v>34.4332785332647</v>
+      </c>
+      <c r="V6" s="12" t="n">
+        <v>35.5167595586671</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="11" t="n">
+        <v>2173754</v>
+      </c>
+      <c r="C7" s="11" t="n">
+        <v>2123839</v>
+      </c>
+      <c r="D7" s="11" t="n">
+        <v>2084794</v>
+      </c>
+      <c r="E7" s="11" t="n">
+        <v>2091319</v>
+      </c>
+      <c r="F7" s="11" t="n">
+        <v>2023029</v>
+      </c>
+      <c r="G7" s="11" t="n">
+        <v>1978447</v>
+      </c>
+      <c r="H7" s="11" t="n">
+        <v>1951799</v>
+      </c>
+      <c r="I7" s="11" t="n">
+        <v>2008381</v>
+      </c>
+      <c r="J7" s="11" t="n">
+        <v>2042392</v>
+      </c>
+      <c r="K7" s="12" t="n">
+        <v>-6.04309411276529</v>
+      </c>
+      <c r="L7" s="17" t="str">
+        <f aca="false">_xlfn.CONCAT(M41," [",N41," ; ",O41,"]")</f>
+        <v>-1.01 [-1.03 ; -0.99]</v>
+      </c>
+      <c r="M7" s="12" t="n">
+        <v>-1.01029393773976</v>
+      </c>
+      <c r="N7" s="12" t="n">
+        <v>-1.02777680240122</v>
+      </c>
+      <c r="O7" s="12" t="n">
+        <v>-0.992807984832467</v>
+      </c>
+      <c r="P7" s="11" t="n">
+        <v>1687241</v>
+      </c>
+      <c r="Q7" s="11" t="n">
+        <v>1804998</v>
+      </c>
+      <c r="R7" s="12" t="n">
+        <v>-11.6233318579391</v>
+      </c>
+      <c r="S7" s="18" t="str">
+        <f aca="false">_xlfn.CONCAT(T41," [",U41," ; ",V41,"]")</f>
+        <v>-6.24 [-6.33 ; -6.14]</v>
+      </c>
+      <c r="T7" s="12" t="n">
+        <v>-6.2354325183736</v>
+      </c>
+      <c r="U7" s="12" t="n">
+        <v>-6.33115549907924</v>
+      </c>
+      <c r="V7" s="12" t="n">
+        <v>-6.1396117155043</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="11" t="n">
+        <v>901122</v>
+      </c>
+      <c r="C8" s="11" t="n">
+        <v>896375</v>
+      </c>
+      <c r="D8" s="11" t="n">
+        <v>909225</v>
+      </c>
+      <c r="E8" s="11" t="n">
+        <v>922278</v>
+      </c>
+      <c r="F8" s="11" t="n">
+        <v>915649</v>
+      </c>
+      <c r="G8" s="11" t="n">
+        <v>912529</v>
+      </c>
+      <c r="H8" s="11" t="n">
+        <v>918994</v>
+      </c>
+      <c r="I8" s="11" t="n">
+        <v>951959</v>
+      </c>
+      <c r="J8" s="11" t="n">
+        <v>981032</v>
+      </c>
+      <c r="K8" s="12" t="n">
+        <v>8.86783365626408</v>
+      </c>
+      <c r="L8" s="17" t="str">
+        <f aca="false">_xlfn.CONCAT(M42," [",N42," ; ",O42,"]")</f>
+        <v>0.9 [0.87 ; 0.93]</v>
+      </c>
+      <c r="M8" s="12" t="n">
+        <v>0.899846520816028</v>
+      </c>
+      <c r="N8" s="12" t="n">
+        <v>0.873274790606637</v>
+      </c>
+      <c r="O8" s="12" t="n">
+        <v>0.926425250469509</v>
+      </c>
+      <c r="P8" s="11" t="n">
+        <v>850860</v>
+      </c>
+      <c r="Q8" s="11" t="n">
+        <v>972436</v>
+      </c>
+      <c r="R8" s="12" t="n">
+        <v>-0.876220143685425</v>
+      </c>
+      <c r="S8" s="18" t="str">
+        <f aca="false">_xlfn.CONCAT(T42," [",U42," ; ",V42,"]")</f>
+        <v>-0.46 [-0.6 ; -0.32]</v>
+      </c>
+      <c r="T8" s="12" t="n">
+        <v>-0.458735496920049</v>
+      </c>
+      <c r="U8" s="12" t="n">
+        <v>-0.601320396241545</v>
+      </c>
+      <c r="V8" s="12" t="n">
+        <v>-0.315946063156092</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="11" t="n">
+        <v>64490</v>
+      </c>
+      <c r="C9" s="11" t="n">
+        <v>66382</v>
+      </c>
+      <c r="D9" s="11" t="n">
+        <v>67188</v>
+      </c>
+      <c r="E9" s="11" t="n">
+        <v>69538</v>
+      </c>
+      <c r="F9" s="11" t="n">
+        <v>70134</v>
+      </c>
+      <c r="G9" s="11" t="n">
+        <v>71008</v>
+      </c>
+      <c r="H9" s="11" t="n">
+        <v>72907</v>
+      </c>
+      <c r="I9" s="11" t="n">
+        <v>75707</v>
+      </c>
+      <c r="J9" s="11" t="n">
+        <v>79418</v>
+      </c>
+      <c r="K9" s="12" t="n">
+        <v>23.1477748488138</v>
+      </c>
+      <c r="L9" s="17" t="str">
+        <f aca="false">_xlfn.CONCAT(M43," [",N43," ; ",O43,"]")</f>
+        <v>2.4 [2.3 ; 2.5]</v>
+      </c>
+      <c r="M9" s="12" t="n">
+        <v>2.39981084746872</v>
+      </c>
+      <c r="N9" s="12" t="n">
+        <v>2.30233557093089</v>
+      </c>
+      <c r="O9" s="12" t="n">
+        <v>2.49737899998521</v>
+      </c>
+      <c r="P9" s="11" t="n">
+        <v>94225</v>
+      </c>
+      <c r="Q9" s="11" t="n">
+        <v>136836</v>
+      </c>
+      <c r="R9" s="12" t="n">
+        <v>72.2984713792843</v>
+      </c>
+      <c r="S9" s="18" t="str">
+        <f aca="false">_xlfn.CONCAT(T43," [",U43," ; ",V43,"]")</f>
+        <v>32.45 [31.87 ; 33.03]</v>
+      </c>
+      <c r="T9" s="12" t="n">
+        <v>32.4503532857293</v>
+      </c>
+      <c r="U9" s="12" t="n">
+        <v>31.8697518368072</v>
+      </c>
+      <c r="V9" s="12" t="n">
+        <v>33.0335110300703</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="11" t="n">
+        <v>836632</v>
+      </c>
+      <c r="C10" s="11" t="n">
+        <v>829993</v>
+      </c>
+      <c r="D10" s="11" t="n">
+        <v>842037</v>
+      </c>
+      <c r="E10" s="11" t="n">
+        <v>852740</v>
+      </c>
+      <c r="F10" s="11" t="n">
+        <v>845515</v>
+      </c>
+      <c r="G10" s="11" t="n">
+        <v>841521</v>
+      </c>
+      <c r="H10" s="11" t="n">
+        <v>846087</v>
+      </c>
+      <c r="I10" s="11" t="n">
+        <v>876252</v>
+      </c>
+      <c r="J10" s="11" t="n">
+        <v>901614</v>
+      </c>
+      <c r="K10" s="12" t="n">
+        <v>7.76709473221201</v>
+      </c>
+      <c r="L10" s="17" t="str">
+        <f aca="false">_xlfn.CONCAT(M44," [",N44," ; ",O44,"]")</f>
+        <v>0.78 [0.75 ; 0.8]</v>
+      </c>
+      <c r="M10" s="12" t="n">
+        <v>0.776457297691069</v>
+      </c>
+      <c r="N10" s="12" t="n">
+        <v>0.748839999702877</v>
+      </c>
+      <c r="O10" s="12" t="n">
+        <v>0.804082166140074</v>
+      </c>
+      <c r="P10" s="11" t="n">
+        <v>756635</v>
+      </c>
+      <c r="Q10" s="11" t="n">
+        <v>835600</v>
+      </c>
+      <c r="R10" s="12" t="n">
+        <v>-7.32175853524901</v>
+      </c>
+      <c r="S10" s="18" t="str">
+        <f aca="false">_xlfn.CONCAT(T44," [",U44," ; ",V44,"]")</f>
+        <v>-3.89 [-4.04 ; -3.75]</v>
+      </c>
+      <c r="T10" s="12" t="n">
+        <v>-3.89381680265861</v>
+      </c>
+      <c r="U10" s="12" t="n">
+        <v>-4.03984981512143</v>
+      </c>
+      <c r="V10" s="12" t="n">
+        <v>-3.7475615558549</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="11" t="n">
+        <v>862065</v>
+      </c>
+      <c r="C11" s="11" t="n">
+        <v>865227</v>
+      </c>
+      <c r="D11" s="11" t="n">
+        <v>887855</v>
+      </c>
+      <c r="E11" s="11" t="n">
+        <v>906238</v>
+      </c>
+      <c r="F11" s="11" t="n">
+        <v>919991</v>
+      </c>
+      <c r="G11" s="11" t="n">
+        <v>932749</v>
+      </c>
+      <c r="H11" s="11" t="n">
+        <v>961355</v>
+      </c>
+      <c r="I11" s="11" t="n">
+        <v>1000323</v>
+      </c>
+      <c r="J11" s="11" t="n">
+        <v>1047103</v>
+      </c>
+      <c r="K11" s="12" t="n">
+        <v>21.464506736731</v>
+      </c>
+      <c r="L11" s="17" t="str">
+        <f aca="false">_xlfn.CONCAT(M45," [",N45," ; ",O45,"]")</f>
+        <v>2.39 [2.36 ; 2.42]</v>
+      </c>
+      <c r="M11" s="12" t="n">
+        <v>2.38998418358811</v>
+      </c>
+      <c r="N11" s="12" t="n">
+        <v>2.36311260185804</v>
+      </c>
+      <c r="O11" s="12" t="n">
+        <v>2.41686281944036</v>
+      </c>
+      <c r="P11" s="11" t="n">
+        <v>922748</v>
+      </c>
+      <c r="Q11" s="11" t="n">
+        <v>1022158</v>
+      </c>
+      <c r="R11" s="12" t="n">
+        <v>-2.3822871293464</v>
+      </c>
+      <c r="S11" s="18" t="str">
+        <f aca="false">_xlfn.CONCAT(T45," [",U45," ; ",V45,"]")</f>
+        <v>-1.24 [-1.38 ; -1.11]</v>
+      </c>
+      <c r="T11" s="12" t="n">
+        <v>-1.24282605509728</v>
+      </c>
+      <c r="U11" s="12" t="n">
+        <v>-1.37978694955467</v>
+      </c>
+      <c r="V11" s="12" t="n">
+        <v>-1.10567495331798</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="11" t="n">
+        <v>74863</v>
+      </c>
+      <c r="C12" s="11" t="n">
+        <v>78292</v>
+      </c>
+      <c r="D12" s="11" t="n">
+        <v>81414</v>
+      </c>
+      <c r="E12" s="11" t="n">
+        <v>86112</v>
+      </c>
+      <c r="F12" s="11" t="n">
+        <v>88426</v>
+      </c>
+      <c r="G12" s="11" t="n">
+        <v>91304</v>
+      </c>
+      <c r="H12" s="11" t="n">
+        <v>96428</v>
+      </c>
+      <c r="I12" s="11" t="n">
+        <v>101911</v>
+      </c>
+      <c r="J12" s="11" t="n">
+        <v>109731</v>
+      </c>
+      <c r="K12" s="12" t="n">
+        <v>46.5757450275837</v>
+      </c>
+      <c r="L12" s="17" t="str">
+        <f aca="false">_xlfn.CONCAT(M46," [",N46," ; ",O46,"]")</f>
+        <v>4.67 [4.59 ; 4.76]</v>
+      </c>
+      <c r="M12" s="12" t="n">
+        <v>4.6747021109371</v>
+      </c>
+      <c r="N12" s="12" t="n">
+        <v>4.58599257604078</v>
+      </c>
+      <c r="O12" s="12" t="n">
+        <v>4.76348688900305</v>
+      </c>
+      <c r="P12" s="11" t="n">
+        <v>131327</v>
+      </c>
+      <c r="Q12" s="11" t="n">
+        <v>164842</v>
+      </c>
+      <c r="R12" s="12" t="n">
+        <v>50.2237289371281</v>
+      </c>
+      <c r="S12" s="18" t="str">
+        <f aca="false">_xlfn.CONCAT(T46," [",U46," ; ",V46,"]")</f>
+        <v>22.76 [22.3 ; 23.23]</v>
+      </c>
+      <c r="T12" s="12" t="n">
+        <v>22.7631784381544</v>
+      </c>
+      <c r="U12" s="12" t="n">
+        <v>22.2966573481554</v>
+      </c>
+      <c r="V12" s="12" t="n">
+        <v>23.2314791510158</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="11" t="n">
+        <v>787202</v>
+      </c>
+      <c r="C13" s="11" t="n">
+        <v>786935</v>
+      </c>
+      <c r="D13" s="11" t="n">
+        <v>806441</v>
+      </c>
+      <c r="E13" s="11" t="n">
+        <v>820126</v>
+      </c>
+      <c r="F13" s="11" t="n">
+        <v>831565</v>
+      </c>
+      <c r="G13" s="11" t="n">
+        <v>841445</v>
+      </c>
+      <c r="H13" s="11" t="n">
+        <v>864927</v>
+      </c>
+      <c r="I13" s="11" t="n">
+        <v>898412</v>
+      </c>
+      <c r="J13" s="11" t="n">
+        <v>937372</v>
+      </c>
+      <c r="K13" s="12" t="n">
+        <v>19.0764251107086</v>
+      </c>
+      <c r="L13" s="17" t="str">
+        <f aca="false">_xlfn.CONCAT(M47," [",N47," ; ",O47,"]")</f>
+        <v>2.15 [2.12 ; 2.18]</v>
+      </c>
+      <c r="M13" s="12" t="n">
+        <v>2.1498062844987</v>
+      </c>
+      <c r="N13" s="12" t="n">
+        <v>2.12160953356761</v>
+      </c>
+      <c r="O13" s="12" t="n">
+        <v>2.17801082082179</v>
+      </c>
+      <c r="P13" s="11" t="n">
+        <v>791421</v>
+      </c>
+      <c r="Q13" s="11" t="n">
+        <v>857316</v>
+      </c>
+      <c r="R13" s="12" t="n">
+        <v>-8.54047272587617</v>
+      </c>
+      <c r="S13" s="18" t="str">
+        <f aca="false">_xlfn.CONCAT(T47," [",U47," ; ",V47,"]")</f>
+        <v>-4.54 [-4.68 ; -4.4]</v>
+      </c>
+      <c r="T13" s="12" t="n">
+        <v>-4.53886019336393</v>
+      </c>
+      <c r="U13" s="12" t="n">
+        <v>-4.68132476176576</v>
+      </c>
+      <c r="V13" s="12" t="n">
+        <v>-4.39618269551044</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="11" t="n">
+        <v>1265005</v>
+      </c>
+      <c r="C14" s="11" t="n">
+        <v>1242813</v>
+      </c>
+      <c r="D14" s="11" t="n">
+        <v>1280887</v>
+      </c>
+      <c r="E14" s="11" t="n">
+        <v>1298632</v>
+      </c>
+      <c r="F14" s="11" t="n">
+        <v>1321753</v>
+      </c>
+      <c r="G14" s="11" t="n">
+        <v>1309646</v>
+      </c>
+      <c r="H14" s="11" t="n">
+        <v>1367428</v>
+      </c>
+      <c r="I14" s="11" t="n">
+        <v>1396091</v>
+      </c>
+      <c r="J14" s="11" t="n">
+        <v>1456559</v>
+      </c>
+      <c r="K14" s="12" t="n">
+        <v>15.1425488436805</v>
+      </c>
+      <c r="L14" s="17" t="str">
+        <f aca="false">_xlfn.CONCAT(M48," [",N48," ; ",O48,"]")</f>
+        <v>1.79 [1.77 ; 1.81]</v>
+      </c>
+      <c r="M14" s="12" t="n">
+        <v>1.78827835008304</v>
+      </c>
+      <c r="N14" s="12" t="n">
+        <v>1.76590439493969</v>
+      </c>
+      <c r="O14" s="12" t="n">
+        <v>1.81065722429894</v>
+      </c>
+      <c r="P14" s="11" t="n">
+        <v>1287629</v>
+      </c>
+      <c r="Q14" s="11" t="n">
+        <v>1384542</v>
+      </c>
+      <c r="R14" s="12" t="n">
+        <v>-4.94432426012266</v>
+      </c>
+      <c r="S14" s="18" t="str">
+        <f aca="false">_xlfn.CONCAT(T48," [",U48," ; ",V48,"]")</f>
+        <v>-2.58 [-2.7 ; -2.47]</v>
+      </c>
+      <c r="T14" s="12" t="n">
+        <v>-2.58279292265582</v>
+      </c>
+      <c r="U14" s="12" t="n">
+        <v>-2.69783029196218</v>
+      </c>
+      <c r="V14" s="12" t="n">
+        <v>-2.46761954819793</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="11" t="n">
+        <v>104694</v>
+      </c>
+      <c r="C15" s="11" t="n">
+        <v>110249</v>
+      </c>
+      <c r="D15" s="11" t="n">
+        <v>117700</v>
+      </c>
+      <c r="E15" s="11" t="n">
+        <v>125940</v>
+      </c>
+      <c r="F15" s="11" t="n">
+        <v>129022</v>
+      </c>
+      <c r="G15" s="11" t="n">
+        <v>131039</v>
+      </c>
+      <c r="H15" s="11" t="n">
+        <v>139745</v>
+      </c>
+      <c r="I15" s="11" t="n">
+        <v>146624</v>
+      </c>
+      <c r="J15" s="11" t="n">
+        <v>158791</v>
+      </c>
+      <c r="K15" s="12" t="n">
+        <v>51.6715380059984</v>
+      </c>
+      <c r="L15" s="17" t="str">
+        <f aca="false">_xlfn.CONCAT(M49," [",N49," ; ",O49,"]")</f>
+        <v>4.96 [4.89 ; 5.04]</v>
+      </c>
+      <c r="M15" s="12" t="n">
+        <v>4.96420459329987</v>
+      </c>
+      <c r="N15" s="12" t="n">
+        <v>4.89001796523099</v>
+      </c>
+      <c r="O15" s="12" t="n">
+        <v>5.03844369209847</v>
+      </c>
+      <c r="P15" s="11" t="n">
+        <v>194346</v>
+      </c>
+      <c r="Q15" s="11" t="n">
+        <v>223313</v>
+      </c>
+      <c r="R15" s="12" t="n">
+        <v>40.6332852617592</v>
+      </c>
+      <c r="S15" s="18" t="str">
+        <f aca="false">_xlfn.CONCAT(T49," [",U49," ; ",V49,"]")</f>
+        <v>18.38 [18 ; 18.75]</v>
+      </c>
+      <c r="T15" s="12" t="n">
+        <v>18.3753144757788</v>
+      </c>
+      <c r="U15" s="12" t="n">
+        <v>17.9989898151775</v>
+      </c>
+      <c r="V15" s="12" t="n">
+        <v>18.7528393182663</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="11" t="n">
+        <v>1160311</v>
+      </c>
+      <c r="C16" s="11" t="n">
+        <v>1132564</v>
+      </c>
+      <c r="D16" s="11" t="n">
+        <v>1163187</v>
+      </c>
+      <c r="E16" s="11" t="n">
+        <v>1172692</v>
+      </c>
+      <c r="F16" s="11" t="n">
+        <v>1192731</v>
+      </c>
+      <c r="G16" s="11" t="n">
+        <v>1178607</v>
+      </c>
+      <c r="H16" s="11" t="n">
+        <v>1227683</v>
+      </c>
+      <c r="I16" s="11" t="n">
+        <v>1249467</v>
+      </c>
+      <c r="J16" s="11" t="n">
+        <v>1297768</v>
+      </c>
+      <c r="K16" s="12" t="n">
+        <v>11.8465652743101</v>
+      </c>
+      <c r="L16" s="17" t="str">
+        <f aca="false">_xlfn.CONCAT(M50," [",N50," ; ",O50,"]")</f>
+        <v>1.45 [1.43 ; 1.48]</v>
+      </c>
+      <c r="M16" s="12" t="n">
+        <v>1.4523064950815</v>
+      </c>
+      <c r="N16" s="12" t="n">
+        <v>1.42883819597275</v>
+      </c>
+      <c r="O16" s="12" t="n">
+        <v>1.4757802242146</v>
+      </c>
+      <c r="P16" s="11" t="n">
+        <v>1093283</v>
+      </c>
+      <c r="Q16" s="11" t="n">
+        <v>1161229</v>
+      </c>
+      <c r="R16" s="12" t="n">
+        <v>-10.5210638573304</v>
+      </c>
+      <c r="S16" s="18" t="str">
+        <f aca="false">_xlfn.CONCAT(T50," [",U50," ; ",V50,"]")</f>
+        <v>-5.61 [-5.73 ; -5.49]</v>
+      </c>
+      <c r="T16" s="12" t="n">
+        <v>-5.60550956159122</v>
+      </c>
+      <c r="U16" s="12" t="n">
+        <v>-5.72575571440454</v>
+      </c>
+      <c r="V16" s="12" t="n">
+        <v>-5.48511003563367</v>
+      </c>
+    </row>
+    <row r="17" s="41" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="9" t="str">
+        <f aca="false">_xlfn.CONCAT(M51," [",N51," ; ",O51,"]")</f>
+        <v>0 [0 ; 0]</v>
+      </c>
+      <c r="M17" s="21"/>
+      <c r="N17" s="21"/>
+      <c r="O17" s="21"/>
+      <c r="P17" s="20"/>
+      <c r="Q17" s="20"/>
+      <c r="R17" s="21"/>
+      <c r="S17" s="13" t="str">
+        <f aca="false">_xlfn.CONCAT(T51," [",U51," ; ",V51,"]")</f>
+        <v>0 [0 ; 0]</v>
+      </c>
+      <c r="T17" s="40"/>
+      <c r="U17" s="40"/>
+      <c r="V17" s="40"/>
+    </row>
+    <row r="18" s="41" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="45"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="45"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="17" t="str">
+        <f aca="false">_xlfn.CONCAT(M52," [",N52," ; ",O52,"]")</f>
+        <v>0 [0 ; 0]</v>
+      </c>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="45"/>
+      <c r="Q18" s="45"/>
+      <c r="R18" s="12"/>
+      <c r="S18" s="18" t="str">
+        <f aca="false">_xlfn.CONCAT(T52," [",U52," ; ",V52,"]")</f>
+        <v>0 [0 ; 0]</v>
+      </c>
+      <c r="T18" s="12"/>
+      <c r="U18" s="12"/>
+      <c r="V18" s="12"/>
+    </row>
+    <row r="19" s="41" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="17" t="str">
+        <f aca="false">_xlfn.CONCAT(M53," [",N53," ; ",O53,"]")</f>
+        <v>0 [0 ; 0]</v>
+      </c>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="12"/>
+      <c r="S19" s="18" t="str">
+        <f aca="false">_xlfn.CONCAT(T53," [",U53," ; ",V53,"]")</f>
+        <v>0 [0 ; 0]</v>
+      </c>
+      <c r="T19" s="12"/>
+      <c r="U19" s="12"/>
+      <c r="V19" s="12"/>
+      <c r="Y19" s="0"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="17" t="str">
+        <f aca="false">_xlfn.CONCAT(M54," [",N54," ; ",O54,"]")</f>
+        <v>0 [0 ; 0]</v>
+      </c>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="12"/>
+      <c r="S20" s="18" t="str">
+        <f aca="false">_xlfn.CONCAT(T54," [",U54," ; ",V54,"]")</f>
+        <v>0 [0 ; 0]</v>
+      </c>
+      <c r="T20" s="12"/>
+      <c r="U20" s="12"/>
+      <c r="V20" s="12"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="45"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="45"/>
+      <c r="I21" s="45"/>
+      <c r="J21" s="45"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="17" t="str">
+        <f aca="false">_xlfn.CONCAT(M55," [",N55," ; ",O55,"]")</f>
+        <v>0 [0 ; 0]</v>
+      </c>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="45"/>
+      <c r="Q21" s="45"/>
+      <c r="R21" s="12"/>
+      <c r="S21" s="18" t="str">
+        <f aca="false">_xlfn.CONCAT(T55," [",U55," ; ",V55,"]")</f>
+        <v>0 [0 ; 0]</v>
+      </c>
+      <c r="T21" s="12"/>
+      <c r="U21" s="12"/>
+      <c r="V21" s="12"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="17" t="str">
+        <f aca="false">_xlfn.CONCAT(M56," [",N56," ; ",O56,"]")</f>
+        <v>0 [0 ; 0]</v>
+      </c>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="12"/>
+      <c r="S22" s="18" t="str">
+        <f aca="false">_xlfn.CONCAT(T56," [",U56," ; ",V56,"]")</f>
+        <v>0 [0 ; 0]</v>
+      </c>
+      <c r="T22" s="12"/>
+      <c r="U22" s="12"/>
+      <c r="V22" s="12"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="17" t="str">
+        <f aca="false">_xlfn.CONCAT(M57," [",N57," ; ",O57,"]")</f>
+        <v>0 [0 ; 0]</v>
+      </c>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="12"/>
+      <c r="S23" s="18" t="str">
+        <f aca="false">_xlfn.CONCAT(T57," [",U57," ; ",V57,"]")</f>
+        <v>0 [0 ; 0]</v>
+      </c>
+      <c r="T23" s="12"/>
+      <c r="U23" s="12"/>
+      <c r="V23" s="12"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="45"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="45"/>
+      <c r="I24" s="45"/>
+      <c r="J24" s="45"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="17" t="str">
+        <f aca="false">_xlfn.CONCAT(M58," [",N58," ; ",O58,"]")</f>
+        <v>0 [0 ; 0]</v>
+      </c>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="45"/>
+      <c r="Q24" s="45"/>
+      <c r="R24" s="12"/>
+      <c r="S24" s="18" t="str">
+        <f aca="false">_xlfn.CONCAT(T58," [",U58," ; ",V58,"]")</f>
+        <v>0 [0 ; 0]</v>
+      </c>
+      <c r="T24" s="12"/>
+      <c r="U24" s="12"/>
+      <c r="V24" s="12"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="17" t="str">
+        <f aca="false">_xlfn.CONCAT(M59," [",N59," ; ",O59,"]")</f>
+        <v>0 [0 ; 0]</v>
+      </c>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="12"/>
+      <c r="S25" s="18" t="str">
+        <f aca="false">_xlfn.CONCAT(T59," [",U59," ; ",V59,"]")</f>
+        <v>0 [0 ; 0]</v>
+      </c>
+      <c r="T25" s="12"/>
+      <c r="U25" s="12"/>
+      <c r="V25" s="12"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="17" t="str">
+        <f aca="false">_xlfn.CONCAT(M60," [",N60," ; ",O60,"]")</f>
+        <v>0 [0 ; 0]</v>
+      </c>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="11"/>
+      <c r="R26" s="12"/>
+      <c r="S26" s="18" t="str">
+        <f aca="false">_xlfn.CONCAT(T60," [",U60," ; ",V60,"]")</f>
+        <v>0 [0 ; 0]</v>
+      </c>
+      <c r="T26" s="12"/>
+      <c r="U26" s="12"/>
+      <c r="V26" s="12"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="45"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="45"/>
+      <c r="J27" s="45"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="17" t="str">
+        <f aca="false">_xlfn.CONCAT(M61," [",N61," ; ",O61,"]")</f>
+        <v>0 [0 ; 0]</v>
+      </c>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="45"/>
+      <c r="Q27" s="45"/>
+      <c r="R27" s="12"/>
+      <c r="S27" s="18" t="str">
+        <f aca="false">_xlfn.CONCAT(T61," [",U61," ; ",V61,"]")</f>
+        <v>0 [0 ; 0]</v>
+      </c>
+      <c r="T27" s="12"/>
+      <c r="U27" s="12"/>
+      <c r="V27" s="12"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="17" t="str">
+        <f aca="false">_xlfn.CONCAT(M62," [",N62," ; ",O62,"]")</f>
+        <v>0 [0 ; 0]</v>
+      </c>
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="12"/>
+      <c r="S28" s="18" t="str">
+        <f aca="false">_xlfn.CONCAT(T62," [",U62," ; ",V62,"]")</f>
+        <v>0 [0 ; 0]</v>
+      </c>
+      <c r="T28" s="12"/>
+      <c r="U28" s="12"/>
+      <c r="V28" s="12"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="17" t="str">
+        <f aca="false">_xlfn.CONCAT(M63," [",N63," ; ",O63,"]")</f>
+        <v>0 [0 ; 0]</v>
+      </c>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
+      <c r="P29" s="11"/>
+      <c r="Q29" s="11"/>
+      <c r="R29" s="12"/>
+      <c r="S29" s="18" t="str">
+        <f aca="false">_xlfn.CONCAT(T63," [",U63," ; ",V63,"]")</f>
+        <v>0 [0 ; 0]</v>
+      </c>
+      <c r="T29" s="12"/>
+      <c r="U29" s="12"/>
+      <c r="V29" s="12"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="48"/>
+      <c r="C30" s="48"/>
+      <c r="D30" s="48"/>
+      <c r="E30" s="48"/>
+      <c r="F30" s="48"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="48"/>
+      <c r="I30" s="48"/>
+      <c r="J30" s="48"/>
+      <c r="K30" s="28"/>
+      <c r="L30" s="29" t="str">
+        <f aca="false">_xlfn.CONCAT(M64," [",N64," ; ",O64,"]")</f>
+        <v>0 [0 ; 0]</v>
+      </c>
+      <c r="M30" s="28"/>
+      <c r="N30" s="28"/>
+      <c r="O30" s="28"/>
+      <c r="P30" s="48"/>
+      <c r="Q30" s="48"/>
+      <c r="R30" s="28"/>
+      <c r="S30" s="32" t="str">
+        <f aca="false">_xlfn.CONCAT(T64," [",U64," ; ",V64,"]")</f>
+        <v>0 [0 ; 0]</v>
+      </c>
+      <c r="T30" s="12"/>
+      <c r="U30" s="12"/>
+      <c r="V30" s="12"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="27"/>
+      <c r="K31" s="28"/>
+      <c r="L31" s="29" t="str">
+        <f aca="false">_xlfn.CONCAT(M65," [",N65," ; ",O65,"]")</f>
+        <v>0 [0 ; 0]</v>
+      </c>
+      <c r="M31" s="28"/>
+      <c r="N31" s="28"/>
+      <c r="O31" s="28"/>
+      <c r="P31" s="27"/>
+      <c r="Q31" s="27"/>
+      <c r="R31" s="28"/>
+      <c r="S31" s="32" t="str">
+        <f aca="false">_xlfn.CONCAT(T65," [",U65," ; ",V65,"]")</f>
+        <v>0 [0 ; 0]</v>
+      </c>
+      <c r="T31" s="12"/>
+      <c r="U31" s="12"/>
+      <c r="V31" s="12"/>
+    </row>
+    <row r="32" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="24"/>
+      <c r="L32" s="24"/>
+      <c r="M32" s="24"/>
+      <c r="N32" s="24"/>
+      <c r="O32" s="24"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="35"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="50"/>
+      <c r="C35" s="50"/>
+      <c r="D35" s="50"/>
+      <c r="E35" s="50"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="50"/>
+      <c r="H35" s="50"/>
+      <c r="I35" s="50"/>
+      <c r="J35" s="50"/>
+      <c r="P35" s="50"/>
+      <c r="Q35" s="50"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="45"/>
+      <c r="C36" s="45"/>
+      <c r="D36" s="45"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="45"/>
+      <c r="G36" s="45"/>
+      <c r="H36" s="45"/>
+      <c r="I36" s="45"/>
+      <c r="J36" s="45"/>
+      <c r="K36" s="45"/>
+      <c r="L36" s="45"/>
+      <c r="M36" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(M2,2),",",".")</f>
+        <v>0.64</v>
+      </c>
+      <c r="N36" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(N2,2),",",".")</f>
+        <v>0.63</v>
+      </c>
+      <c r="O36" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(O2,2),",",".")</f>
+        <v>0.65</v>
+      </c>
+      <c r="P36" s="45"/>
+      <c r="Q36" s="45"/>
+      <c r="T36" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(T2,2),",",".")</f>
+        <v>-2.52</v>
+      </c>
+      <c r="U36" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(U2,2),",",".")</f>
+        <v>-2.58</v>
+      </c>
+      <c r="V36" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(V2,2),",",".")</f>
+        <v>-2.46</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="45"/>
+      <c r="C37" s="45"/>
+      <c r="D37" s="45"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="45"/>
+      <c r="G37" s="45"/>
+      <c r="H37" s="45"/>
+      <c r="I37" s="45"/>
+      <c r="J37" s="45"/>
+      <c r="K37" s="45"/>
+      <c r="L37" s="45"/>
+      <c r="M37" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(M3,2),",",".")</f>
+        <v>3.54</v>
+      </c>
+      <c r="N37" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(N3,2),",",".")</f>
+        <v>3.5</v>
+      </c>
+      <c r="O37" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(O3,2),",",".")</f>
+        <v>3.58</v>
+      </c>
+      <c r="P37" s="45"/>
+      <c r="Q37" s="45"/>
+      <c r="T37" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(T3,2),",",".")</f>
+        <v>25.56</v>
+      </c>
+      <c r="U37" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(U3,2),",",".")</f>
+        <v>25.32</v>
+      </c>
+      <c r="V37" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(V3,2),",",".")</f>
+        <v>25.79</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="50"/>
+      <c r="C38" s="50"/>
+      <c r="D38" s="50"/>
+      <c r="E38" s="50"/>
+      <c r="F38" s="50"/>
+      <c r="G38" s="50"/>
+      <c r="H38" s="50"/>
+      <c r="I38" s="50"/>
+      <c r="J38" s="50"/>
+      <c r="K38" s="45"/>
+      <c r="L38" s="45"/>
+      <c r="M38" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(M4,2),",",".")</f>
+        <v>0.42</v>
+      </c>
+      <c r="N38" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(N4,2),",",".")</f>
+        <v>0.41</v>
+      </c>
+      <c r="O38" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(O4,2),",",".")</f>
+        <v>0.43</v>
+      </c>
+      <c r="P38" s="50"/>
+      <c r="Q38" s="50"/>
+      <c r="T38" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(T4,2),",",".")</f>
+        <v>-5.36</v>
+      </c>
+      <c r="U38" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(U4,2),",",".")</f>
+        <v>-5.42</v>
+      </c>
+      <c r="V38" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(V4,2),",",".")</f>
+        <v>-5.3</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="45"/>
+      <c r="C39" s="45"/>
+      <c r="D39" s="45"/>
+      <c r="E39" s="45"/>
+      <c r="F39" s="45"/>
+      <c r="G39" s="45"/>
+      <c r="H39" s="45"/>
+      <c r="I39" s="45"/>
+      <c r="J39" s="45"/>
+      <c r="K39" s="45"/>
+      <c r="L39" s="45"/>
+      <c r="M39" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(M5,2),",",".")</f>
+        <v>-0.92</v>
+      </c>
+      <c r="N39" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(N5,2),",",".")</f>
+        <v>-0.94</v>
+      </c>
+      <c r="O39" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(O5,2),",",".")</f>
+        <v>-0.9</v>
+      </c>
+      <c r="P39" s="45"/>
+      <c r="Q39" s="45"/>
+      <c r="T39" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(T5,2),",",".")</f>
+        <v>-4.07</v>
+      </c>
+      <c r="U39" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(U5,2),",",".")</f>
+        <v>-4.17</v>
+      </c>
+      <c r="V39" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(V5,2),",",".")</f>
+        <v>-3.98</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="51"/>
+      <c r="C40" s="51"/>
+      <c r="D40" s="51"/>
+      <c r="E40" s="51"/>
+      <c r="F40" s="51"/>
+      <c r="G40" s="51"/>
+      <c r="H40" s="51"/>
+      <c r="I40" s="51"/>
+      <c r="J40" s="51"/>
+      <c r="K40" s="51"/>
+      <c r="L40" s="51"/>
+      <c r="M40" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(M6,2),",",".")</f>
+        <v>1.23</v>
+      </c>
+      <c r="N40" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(N6,2),",",".")</f>
+        <v>1.14</v>
+      </c>
+      <c r="O40" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(O6,2),",",".")</f>
+        <v>1.32</v>
+      </c>
+      <c r="P40" s="51"/>
+      <c r="Q40" s="51"/>
+      <c r="T40" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(T6,2),",",".")</f>
+        <v>34.97</v>
+      </c>
+      <c r="U40" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(U6,2),",",".")</f>
+        <v>34.43</v>
+      </c>
+      <c r="V40" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(V6,2),",",".")</f>
+        <v>35.52</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="50"/>
+      <c r="C41" s="50"/>
+      <c r="D41" s="50"/>
+      <c r="E41" s="50"/>
+      <c r="F41" s="50"/>
+      <c r="G41" s="50"/>
+      <c r="H41" s="50"/>
+      <c r="I41" s="50"/>
+      <c r="J41" s="50"/>
+      <c r="K41" s="51"/>
+      <c r="L41" s="51"/>
+      <c r="M41" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(M7,2),",",".")</f>
+        <v>-1.01</v>
+      </c>
+      <c r="N41" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(N7,2),",",".")</f>
+        <v>-1.03</v>
+      </c>
+      <c r="O41" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(O7,2),",",".")</f>
+        <v>-0.99</v>
+      </c>
+      <c r="P41" s="50"/>
+      <c r="Q41" s="50"/>
+      <c r="T41" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(T7,2),",",".")</f>
+        <v>-6.24</v>
+      </c>
+      <c r="U41" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(U7,2),",",".")</f>
+        <v>-6.33</v>
+      </c>
+      <c r="V41" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(V7,2),",",".")</f>
+        <v>-6.14</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="45"/>
+      <c r="C42" s="45"/>
+      <c r="D42" s="45"/>
+      <c r="E42" s="45"/>
+      <c r="F42" s="45"/>
+      <c r="G42" s="45"/>
+      <c r="H42" s="45"/>
+      <c r="I42" s="45"/>
+      <c r="J42" s="45"/>
+      <c r="K42" s="51"/>
+      <c r="L42" s="51"/>
+      <c r="M42" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(M8,2),",",".")</f>
+        <v>0.9</v>
+      </c>
+      <c r="N42" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(N8,2),",",".")</f>
+        <v>0.87</v>
+      </c>
+      <c r="O42" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(O8,2),",",".")</f>
+        <v>0.93</v>
+      </c>
+      <c r="P42" s="45"/>
+      <c r="Q42" s="45"/>
+      <c r="T42" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(T8,2),",",".")</f>
+        <v>-0.46</v>
+      </c>
+      <c r="U42" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(U8,2),",",".")</f>
+        <v>-0.6</v>
+      </c>
+      <c r="V42" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(V8,2),",",".")</f>
+        <v>-0.32</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="51"/>
+      <c r="C43" s="51"/>
+      <c r="D43" s="51"/>
+      <c r="E43" s="51"/>
+      <c r="F43" s="51"/>
+      <c r="G43" s="51"/>
+      <c r="H43" s="51"/>
+      <c r="I43" s="51"/>
+      <c r="J43" s="51"/>
+      <c r="K43" s="51"/>
+      <c r="L43" s="51"/>
+      <c r="M43" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(M9,2),",",".")</f>
+        <v>2.4</v>
+      </c>
+      <c r="N43" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(N9,2),",",".")</f>
+        <v>2.3</v>
+      </c>
+      <c r="O43" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(O9,2),",",".")</f>
+        <v>2.5</v>
+      </c>
+      <c r="P43" s="51"/>
+      <c r="Q43" s="51"/>
+      <c r="T43" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(T9,2),",",".")</f>
+        <v>32.45</v>
+      </c>
+      <c r="U43" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(U9,2),",",".")</f>
+        <v>31.87</v>
+      </c>
+      <c r="V43" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(V9,2),",",".")</f>
+        <v>33.03</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="50"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="50"/>
+      <c r="E44" s="50"/>
+      <c r="F44" s="50"/>
+      <c r="G44" s="50"/>
+      <c r="H44" s="50"/>
+      <c r="I44" s="50"/>
+      <c r="J44" s="50"/>
+      <c r="K44" s="51"/>
+      <c r="L44" s="51"/>
+      <c r="M44" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(M10,2),",",".")</f>
+        <v>0.78</v>
+      </c>
+      <c r="N44" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(N10,2),",",".")</f>
+        <v>0.75</v>
+      </c>
+      <c r="O44" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(O10,2),",",".")</f>
+        <v>0.8</v>
+      </c>
+      <c r="P44" s="50"/>
+      <c r="Q44" s="50"/>
+      <c r="T44" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(T10,2),",",".")</f>
+        <v>-3.89</v>
+      </c>
+      <c r="U44" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(U10,2),",",".")</f>
+        <v>-4.04</v>
+      </c>
+      <c r="V44" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(V10,2),",",".")</f>
+        <v>-3.75</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="45"/>
+      <c r="C45" s="45"/>
+      <c r="D45" s="45"/>
+      <c r="E45" s="45"/>
+      <c r="F45" s="45"/>
+      <c r="G45" s="45"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="45"/>
+      <c r="J45" s="45"/>
+      <c r="K45" s="51"/>
+      <c r="L45" s="51"/>
+      <c r="M45" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(M11,2),",",".")</f>
+        <v>2.39</v>
+      </c>
+      <c r="N45" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(N11,2),",",".")</f>
+        <v>2.36</v>
+      </c>
+      <c r="O45" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(O11,2),",",".")</f>
+        <v>2.42</v>
+      </c>
+      <c r="P45" s="45"/>
+      <c r="Q45" s="45"/>
+      <c r="T45" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(T11,2),",",".")</f>
+        <v>-1.24</v>
+      </c>
+      <c r="U45" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(U11,2),",",".")</f>
+        <v>-1.38</v>
+      </c>
+      <c r="V45" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(V11,2),",",".")</f>
+        <v>-1.11</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="51"/>
+      <c r="C46" s="51"/>
+      <c r="D46" s="51"/>
+      <c r="E46" s="51"/>
+      <c r="F46" s="51"/>
+      <c r="G46" s="51"/>
+      <c r="H46" s="51"/>
+      <c r="I46" s="51"/>
+      <c r="J46" s="51"/>
+      <c r="K46" s="51"/>
+      <c r="L46" s="51"/>
+      <c r="M46" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(M12,2),",",".")</f>
+        <v>4.67</v>
+      </c>
+      <c r="N46" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(N12,2),",",".")</f>
+        <v>4.59</v>
+      </c>
+      <c r="O46" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(O12,2),",",".")</f>
+        <v>4.76</v>
+      </c>
+      <c r="P46" s="51"/>
+      <c r="Q46" s="51"/>
+      <c r="T46" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(T12,2),",",".")</f>
+        <v>22.76</v>
+      </c>
+      <c r="U46" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(U12,2),",",".")</f>
+        <v>22.3</v>
+      </c>
+      <c r="V46" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(V12,2),",",".")</f>
+        <v>23.23</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="50"/>
+      <c r="C47" s="50"/>
+      <c r="D47" s="50"/>
+      <c r="E47" s="50"/>
+      <c r="F47" s="50"/>
+      <c r="G47" s="50"/>
+      <c r="H47" s="50"/>
+      <c r="I47" s="50"/>
+      <c r="J47" s="50"/>
+      <c r="K47" s="51"/>
+      <c r="L47" s="51"/>
+      <c r="M47" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(M13,2),",",".")</f>
+        <v>2.15</v>
+      </c>
+      <c r="N47" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(N13,2),",",".")</f>
+        <v>2.12</v>
+      </c>
+      <c r="O47" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(O13,2),",",".")</f>
+        <v>2.18</v>
+      </c>
+      <c r="P47" s="50"/>
+      <c r="Q47" s="50"/>
+      <c r="T47" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(T13,2),",",".")</f>
+        <v>-4.54</v>
+      </c>
+      <c r="U47" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(U13,2),",",".")</f>
+        <v>-4.68</v>
+      </c>
+      <c r="V47" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(V13,2),",",".")</f>
+        <v>-4.4</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="45"/>
+      <c r="C48" s="45"/>
+      <c r="D48" s="45"/>
+      <c r="E48" s="45"/>
+      <c r="F48" s="45"/>
+      <c r="G48" s="45"/>
+      <c r="H48" s="45"/>
+      <c r="I48" s="45"/>
+      <c r="J48" s="45"/>
+      <c r="K48" s="51"/>
+      <c r="L48" s="51"/>
+      <c r="M48" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(M14,2),",",".")</f>
+        <v>1.79</v>
+      </c>
+      <c r="N48" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(N14,2),",",".")</f>
+        <v>1.77</v>
+      </c>
+      <c r="O48" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(O14,2),",",".")</f>
+        <v>1.81</v>
+      </c>
+      <c r="P48" s="45"/>
+      <c r="Q48" s="45"/>
+      <c r="T48" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(T14,2),",",".")</f>
+        <v>-2.58</v>
+      </c>
+      <c r="U48" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(U14,2),",",".")</f>
+        <v>-2.7</v>
+      </c>
+      <c r="V48" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(V14,2),",",".")</f>
+        <v>-2.47</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="51"/>
+      <c r="C49" s="51"/>
+      <c r="D49" s="51"/>
+      <c r="E49" s="51"/>
+      <c r="F49" s="51"/>
+      <c r="G49" s="51"/>
+      <c r="H49" s="51"/>
+      <c r="I49" s="51"/>
+      <c r="J49" s="51"/>
+      <c r="K49" s="51"/>
+      <c r="L49" s="51"/>
+      <c r="M49" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(M15,2),",",".")</f>
+        <v>4.96</v>
+      </c>
+      <c r="N49" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(N15,2),",",".")</f>
+        <v>4.89</v>
+      </c>
+      <c r="O49" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(O15,2),",",".")</f>
+        <v>5.04</v>
+      </c>
+      <c r="P49" s="45"/>
+      <c r="Q49" s="45"/>
+      <c r="T49" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(T15,2),",",".")</f>
+        <v>18.38</v>
+      </c>
+      <c r="U49" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(U15,2),",",".")</f>
+        <v>18</v>
+      </c>
+      <c r="V49" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(V15,2),",",".")</f>
+        <v>18.75</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="51"/>
+      <c r="C50" s="51"/>
+      <c r="D50" s="51"/>
+      <c r="E50" s="51"/>
+      <c r="F50" s="51"/>
+      <c r="G50" s="51"/>
+      <c r="H50" s="51"/>
+      <c r="I50" s="51"/>
+      <c r="J50" s="51"/>
+      <c r="K50" s="51"/>
+      <c r="L50" s="51"/>
+      <c r="M50" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(M16,2),",",".")</f>
+        <v>1.45</v>
+      </c>
+      <c r="N50" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(N16,2),",",".")</f>
+        <v>1.43</v>
+      </c>
+      <c r="O50" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(O16,2),",",".")</f>
+        <v>1.48</v>
+      </c>
+      <c r="P50" s="45"/>
+      <c r="Q50" s="45"/>
+      <c r="T50" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(T16,2),",",".")</f>
+        <v>-5.61</v>
+      </c>
+      <c r="U50" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(U16,2),",",".")</f>
+        <v>-5.73</v>
+      </c>
+      <c r="V50" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(V16,2),",",".")</f>
+        <v>-5.49</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="51"/>
+      <c r="C51" s="51"/>
+      <c r="D51" s="51"/>
+      <c r="E51" s="51"/>
+      <c r="F51" s="51"/>
+      <c r="G51" s="51"/>
+      <c r="H51" s="51"/>
+      <c r="I51" s="51"/>
+      <c r="J51" s="51"/>
+      <c r="K51" s="51"/>
+      <c r="L51" s="51"/>
+      <c r="M51" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(M17,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="N51" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(N17,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="O51" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(O17,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="P51" s="45"/>
+      <c r="Q51" s="45"/>
+      <c r="T51" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(T17,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="U51" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(U17,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="V51" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(V17,2),",",".")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="51"/>
+      <c r="C52" s="51"/>
+      <c r="D52" s="51"/>
+      <c r="E52" s="51"/>
+      <c r="F52" s="51"/>
+      <c r="G52" s="51"/>
+      <c r="H52" s="51"/>
+      <c r="I52" s="51"/>
+      <c r="J52" s="51"/>
+      <c r="K52" s="51"/>
+      <c r="L52" s="51"/>
+      <c r="M52" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(M18,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="N52" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(N18,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="O52" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(O18,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="P52" s="45"/>
+      <c r="Q52" s="45"/>
+      <c r="T52" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(T18,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="U52" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(U18,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="V52" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(V18,2),",",".")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M53" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(M19,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="N53" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(N19,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="O53" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(O19,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="P53" s="45"/>
+      <c r="Q53" s="45"/>
+      <c r="T53" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(T19,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="U53" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(U19,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="V53" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(V19,2),",",".")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M54" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(M20,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="N54" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(N20,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="O54" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(O20,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="P54" s="45"/>
+      <c r="Q54" s="45"/>
+      <c r="T54" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(T20,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="U54" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(U20,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="V54" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(V20,2),",",".")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M55" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(M21,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="N55" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(N21,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="O55" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(O21,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="P55" s="45"/>
+      <c r="Q55" s="45"/>
+      <c r="T55" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(T21,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="U55" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(U21,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="V55" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(V21,2),",",".")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M56" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(M22,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="N56" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(N22,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="O56" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(O22,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="P56" s="45"/>
+      <c r="Q56" s="45"/>
+      <c r="T56" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(T22,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="U56" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(U22,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="V56" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(V22,2),",",".")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M57" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(M23,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="N57" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(N23,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="O57" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(O23,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="P57" s="45"/>
+      <c r="Q57" s="45"/>
+      <c r="T57" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(T23,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="U57" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(U23,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="V57" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(V23,2),",",".")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M58" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(M24,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="N58" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(N24,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="O58" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(O24,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="P58" s="45"/>
+      <c r="Q58" s="45"/>
+      <c r="T58" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(T24,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="U58" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(U24,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="V58" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(V24,2),",",".")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M59" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(M25,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="N59" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(N25,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="O59" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(O25,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="P59" s="45"/>
+      <c r="Q59" s="45"/>
+      <c r="T59" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(T25,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="U59" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(U25,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="V59" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(V25,2),",",".")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M60" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(M26,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="N60" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(N26,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="O60" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(O26,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="P60" s="45"/>
+      <c r="Q60" s="45"/>
+      <c r="T60" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(T26,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="U60" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(U26,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="V60" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(V26,2),",",".")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M61" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(M27,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="N61" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(N27,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="O61" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(O27,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="P61" s="45"/>
+      <c r="Q61" s="45"/>
+      <c r="T61" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(T27,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="U61" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(U27,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="V61" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(V27,2),",",".")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M62" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(M28,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="N62" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(N28,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="O62" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(O28,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="P62" s="45"/>
+      <c r="Q62" s="45"/>
+      <c r="T62" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(T28,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="U62" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(U28,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="V62" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(V28,2),",",".")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M63" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(M29,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="N63" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(N29,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="O63" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(O29,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="P63" s="45"/>
+      <c r="Q63" s="45"/>
+      <c r="T63" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(T29,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="U63" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(U29,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="V63" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(V29,2),",",".")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M64" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(M30,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="N64" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(N30,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="O64" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(O30,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="P64" s="45"/>
+      <c r="Q64" s="45"/>
+      <c r="T64" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(T30,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="U64" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(U30,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="V64" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(V30,2),",",".")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M65" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(M31,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="N65" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(N31,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="O65" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(O31,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="P65" s="45"/>
+      <c r="Q65" s="45"/>
+      <c r="T65" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(T31,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="U65" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(U31,2),",",".")</f>
+        <v>0</v>
+      </c>
+      <c r="V65" s="45" t="str">
+        <f aca="false">SUBSTITUTE(ROUND(V31,2),",",".")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M66" s="45"/>
+      <c r="N66" s="45"/>
+      <c r="O66" s="45"/>
+      <c r="P66" s="45"/>
+      <c r="Q66" s="45"/>
+      <c r="T66" s="45"/>
+      <c r="U66" s="45"/>
+      <c r="V66" s="45"/>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M67" s="45"/>
+      <c r="N67" s="45"/>
+      <c r="O67" s="45"/>
+      <c r="P67" s="45"/>
+      <c r="Q67" s="45"/>
+      <c r="T67" s="45"/>
+      <c r="U67" s="45"/>
+      <c r="V67" s="45"/>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M68" s="45"/>
+      <c r="N68" s="45"/>
+      <c r="O68" s="45"/>
+      <c r="P68" s="45"/>
+      <c r="Q68" s="45"/>
+      <c r="T68" s="45"/>
+      <c r="U68" s="45"/>
+      <c r="V68" s="45"/>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M69" s="45"/>
+      <c r="N69" s="45"/>
+      <c r="O69" s="45"/>
+      <c r="P69" s="45"/>
+      <c r="Q69" s="45"/>
+      <c r="T69" s="45"/>
+      <c r="U69" s="45"/>
+      <c r="V69" s="45"/>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M70" s="45"/>
+      <c r="N70" s="45"/>
+      <c r="O70" s="45"/>
+      <c r="P70" s="45"/>
+      <c r="Q70" s="45"/>
+      <c r="T70" s="45"/>
+      <c r="U70" s="45"/>
+      <c r="V70" s="45"/>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M71" s="45"/>
+      <c r="N71" s="45"/>
+      <c r="O71" s="45"/>
+      <c r="P71" s="45"/>
+      <c r="Q71" s="45"/>
+      <c r="T71" s="45"/>
+      <c r="U71" s="45"/>
+      <c r="V71" s="45"/>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M72" s="45"/>
+      <c r="N72" s="45"/>
+      <c r="O72" s="45"/>
+      <c r="T72" s="45"/>
+      <c r="U72" s="45"/>
+      <c r="V72" s="45"/>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M73" s="45"/>
+      <c r="N73" s="45"/>
+      <c r="O73" s="45"/>
+      <c r="T73" s="45"/>
+      <c r="U73" s="45"/>
+      <c r="V73" s="45"/>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M74" s="45"/>
+      <c r="N74" s="45"/>
+      <c r="O74" s="45"/>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M75" s="45"/>
+      <c r="N75" s="45"/>
+      <c r="O75" s="45"/>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M76" s="45"/>
+      <c r="N76" s="45"/>
+      <c r="O76" s="45"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="0" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>